<commit_message>
change hasPart to HasPart, fix date formats
</commit_message>
<xml_diff>
--- a/EEE2000-metadata_mapping.xlsx
+++ b/EEE2000-metadata_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amw23\Documents\GitHub\cci_data_bridge_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajw22/git/cci_data_bridge_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3529F200-EAE9-41A4-B325-5F8B99981D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9457B80D-5CB3-C147-BF63-B203017DCB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B9DA58AC-C110-4CBA-A19B-6F37B44EEA38}"/>
+    <workbookView xWindow="-31720" yWindow="1160" windowWidth="28800" windowHeight="15840" xr2:uid="{B9DA58AC-C110-4CBA-A19B-6F37B44EEA38}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1593" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="368">
   <si>
     <t>Dataset 1</t>
   </si>
@@ -949,9 +949,6 @@
     <t>Indicates A is replaced by B</t>
   </si>
   <si>
-    <t>2022-31-12</t>
-  </si>
-  <si>
     <t>variable=[mass_concentration of chlorophyll_a,remote_sensing_reflectance],
 projection=regular_latitude_longitude_grid,
 version=6_0</t>
@@ -998,12 +995,6 @@
   </si>
   <si>
     <t>CCI product has data up until 2017-2018, while C3S product has data from 2017-2020.   C3S product is a newer version (version depends on date range)</t>
-  </si>
-  <si>
-    <t>2021-09-31</t>
-  </si>
-  <si>
-    <t>2018-09-31</t>
   </si>
   <si>
     <t>time_aggregation=5_daily_composite,
@@ -1089,10 +1080,6 @@
   </si>
   <si>
     <t>CCI data is a subset of the C3S data</t>
-  </si>
-  <si>
-    <t>hasPart,
-IsNewVersionOf</t>
   </si>
   <si>
     <t>CCI data is a subset of the C3S aerosol dataset.  C3S data is a newer version</t>
@@ -1890,28 +1877,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC0B67C-1229-4907-A814-DF79422D0B81}">
   <dimension ref="A1:M160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D145" workbookViewId="0">
-      <selection activeCell="J148" sqref="J148"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="C148" sqref="C148"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="42.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="23.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="30.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="30.5" style="13" customWidth="1"/>
+    <col min="9" max="9" width="42.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.1640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1933,7 +1920,7 @@
       <c r="K1" s="3"/>
       <c r="M1" s="18"/>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1970,7 +1957,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2011,7 +1998,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2052,7 +2039,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -2093,11 +2080,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
     </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2135,10 +2122,10 @@
         <v>34</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -2176,10 +2163,10 @@
         <v>34</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -2217,10 +2204,10 @@
         <v>34</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
@@ -2258,10 +2245,10 @@
         <v>34</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2299,10 +2286,10 @@
         <v>34</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
@@ -2340,14 +2327,14 @@
         <v>34</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
     </row>
-    <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -2373,7 +2360,7 @@
         <v>46</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J14" s="4" t="s">
         <v>47</v>
@@ -2388,7 +2375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -2414,7 +2401,7 @@
         <v>51</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>14</v>
@@ -2426,10 +2413,10 @@
         <v>45</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -2455,7 +2442,7 @@
         <v>51</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>33</v>
@@ -2467,10 +2454,10 @@
         <v>45</v>
       </c>
       <c r="M16" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2496,7 +2483,7 @@
         <v>51</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>33</v>
@@ -2508,10 +2495,10 @@
         <v>45</v>
       </c>
       <c r="M17" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -2549,10 +2536,10 @@
         <v>45</v>
       </c>
       <c r="M18" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -2578,7 +2565,7 @@
         <v>51</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>33</v>
@@ -2590,10 +2577,10 @@
         <v>45</v>
       </c>
       <c r="M19" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2619,7 +2606,7 @@
         <v>51</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>33</v>
@@ -2631,10 +2618,10 @@
         <v>45</v>
       </c>
       <c r="M20" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2660,7 +2647,7 @@
         <v>51</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>33</v>
@@ -2672,10 +2659,10 @@
         <v>45</v>
       </c>
       <c r="M21" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -2701,7 +2688,7 @@
         <v>54</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>33</v>
@@ -2713,10 +2700,10 @@
         <v>45</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -2742,7 +2729,7 @@
         <v>51</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>55</v>
@@ -2754,10 +2741,10 @@
         <v>45</v>
       </c>
       <c r="M23" s="9" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2783,7 +2770,7 @@
         <v>51</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>33</v>
@@ -2795,10 +2782,10 @@
         <v>45</v>
       </c>
       <c r="M24" s="9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -2824,7 +2811,7 @@
         <v>46</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>59</v>
@@ -2836,10 +2823,10 @@
         <v>45</v>
       </c>
       <c r="M25" s="9" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -2865,7 +2852,7 @@
         <v>50</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>33</v>
@@ -2877,10 +2864,10 @@
         <v>45</v>
       </c>
       <c r="M26" s="9" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -2906,7 +2893,7 @@
         <v>50</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>33</v>
@@ -2918,10 +2905,10 @@
         <v>45</v>
       </c>
       <c r="M27" s="9" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>49</v>
       </c>
@@ -2947,7 +2934,7 @@
         <v>50</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>33</v>
@@ -2959,10 +2946,10 @@
         <v>45</v>
       </c>
       <c r="M28" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>49</v>
       </c>
@@ -2988,7 +2975,7 @@
         <v>51</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>63</v>
@@ -3000,10 +2987,10 @@
         <v>45</v>
       </c>
       <c r="M29" s="9" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -3029,7 +3016,7 @@
         <v>51</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>64</v>
@@ -3041,10 +3028,10 @@
         <v>45</v>
       </c>
       <c r="M30" s="9" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -3070,7 +3057,7 @@
         <v>51</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>65</v>
@@ -3082,10 +3069,10 @@
         <v>45</v>
       </c>
       <c r="M31" s="9" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -3111,7 +3098,7 @@
         <v>51</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>66</v>
@@ -3123,10 +3110,10 @@
         <v>45</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -3152,7 +3139,7 @@
         <v>51</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J33" s="4" t="s">
         <v>67</v>
@@ -3164,10 +3151,10 @@
         <v>45</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -3193,7 +3180,7 @@
         <v>51</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>68</v>
@@ -3205,10 +3192,10 @@
         <v>45</v>
       </c>
       <c r="M34" s="9" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -3234,7 +3221,7 @@
         <v>50</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>33</v>
@@ -3246,10 +3233,10 @@
         <v>45</v>
       </c>
       <c r="M35" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -3275,7 +3262,7 @@
         <v>50</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J36" s="4" t="s">
         <v>33</v>
@@ -3287,10 +3274,10 @@
         <v>45</v>
       </c>
       <c r="M36" s="9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -3316,7 +3303,7 @@
         <v>50</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J37" s="4" t="s">
         <v>33</v>
@@ -3328,10 +3315,10 @@
         <v>45</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -3369,10 +3356,10 @@
         <v>45</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -3410,10 +3397,10 @@
         <v>45</v>
       </c>
       <c r="M39" s="9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -3451,10 +3438,10 @@
         <v>45</v>
       </c>
       <c r="M40" s="9" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -3492,10 +3479,10 @@
         <v>45</v>
       </c>
       <c r="M41" s="9" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>49</v>
       </c>
@@ -3533,10 +3520,10 @@
         <v>45</v>
       </c>
       <c r="M42" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -3574,10 +3561,10 @@
         <v>45</v>
       </c>
       <c r="M43" s="9" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -3615,10 +3602,10 @@
         <v>45</v>
       </c>
       <c r="M44" s="9" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -3656,10 +3643,10 @@
         <v>45</v>
       </c>
       <c r="M45" s="9" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>49</v>
       </c>
@@ -3697,10 +3684,10 @@
         <v>45</v>
       </c>
       <c r="M46" s="9" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -3738,10 +3725,10 @@
         <v>45</v>
       </c>
       <c r="M47" s="9" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -3779,10 +3766,10 @@
         <v>45</v>
       </c>
       <c r="M48" s="9" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -3820,10 +3807,10 @@
         <v>45</v>
       </c>
       <c r="M49" s="9" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -3861,10 +3848,10 @@
         <v>45</v>
       </c>
       <c r="M50" s="9" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -3902,10 +3889,10 @@
         <v>45</v>
       </c>
       <c r="M51" s="9" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -3943,10 +3930,10 @@
         <v>45</v>
       </c>
       <c r="M52" s="9" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -3984,10 +3971,10 @@
         <v>45</v>
       </c>
       <c r="M53" s="9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -4025,10 +4012,10 @@
         <v>45</v>
       </c>
       <c r="M54" s="9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -4066,10 +4053,10 @@
         <v>45</v>
       </c>
       <c r="M55" s="9" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -4098,7 +4085,7 @@
         <v>73</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="K56" t="s">
         <v>20</v>
@@ -4107,10 +4094,10 @@
         <v>45</v>
       </c>
       <c r="M56" s="9" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -4139,7 +4126,7 @@
         <v>73</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="K57" t="s">
         <v>20</v>
@@ -4148,10 +4135,10 @@
         <v>45</v>
       </c>
       <c r="M57" s="9" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>49</v>
       </c>
@@ -4189,10 +4176,10 @@
         <v>45</v>
       </c>
       <c r="M58" s="9" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>49</v>
       </c>
@@ -4230,10 +4217,10 @@
         <v>45</v>
       </c>
       <c r="M59" s="9" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -4271,10 +4258,10 @@
         <v>45</v>
       </c>
       <c r="M60" s="9" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>49</v>
       </c>
@@ -4312,10 +4299,10 @@
         <v>45</v>
       </c>
       <c r="M61" s="9" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>49</v>
       </c>
@@ -4344,7 +4331,7 @@
         <v>73</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="K62" t="s">
         <v>20</v>
@@ -4353,10 +4340,10 @@
         <v>45</v>
       </c>
       <c r="M62" s="9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>49</v>
       </c>
@@ -4385,7 +4372,7 @@
         <v>73</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="K63" t="s">
         <v>20</v>
@@ -4394,10 +4381,10 @@
         <v>45</v>
       </c>
       <c r="M63" s="9" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>49</v>
       </c>
@@ -4426,7 +4413,7 @@
         <v>73</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="K64" t="s">
         <v>20</v>
@@ -4435,10 +4422,10 @@
         <v>45</v>
       </c>
       <c r="M64" s="9" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>49</v>
       </c>
@@ -4467,7 +4454,7 @@
         <v>73</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="K65" t="s">
         <v>20</v>
@@ -4476,10 +4463,10 @@
         <v>45</v>
       </c>
       <c r="M65" s="9" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -4508,7 +4495,7 @@
         <v>73</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="K66" t="s">
         <v>20</v>
@@ -4517,10 +4504,10 @@
         <v>45</v>
       </c>
       <c r="M66" s="9" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>49</v>
       </c>
@@ -4549,7 +4536,7 @@
         <v>73</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K67" t="s">
         <v>20</v>
@@ -4558,10 +4545,10 @@
         <v>45</v>
       </c>
       <c r="M67" s="9" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>49</v>
       </c>
@@ -4590,7 +4577,7 @@
         <v>73</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="K68" t="s">
         <v>20</v>
@@ -4599,10 +4586,10 @@
         <v>45</v>
       </c>
       <c r="M68" s="9" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>49</v>
       </c>
@@ -4631,7 +4618,7 @@
         <v>73</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="K69" t="s">
         <v>20</v>
@@ -4640,10 +4627,10 @@
         <v>45</v>
       </c>
       <c r="M69" s="9" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>49</v>
       </c>
@@ -4681,10 +4668,10 @@
         <v>45</v>
       </c>
       <c r="M70" s="9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>49</v>
       </c>
@@ -4722,14 +4709,14 @@
         <v>45</v>
       </c>
       <c r="M71" s="9" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B72" s="20"/>
       <c r="C72" s="20"/>
     </row>
-    <row r="73" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>97</v>
       </c>
@@ -4749,13 +4736,13 @@
         <v>98</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H73" s="13" t="s">
         <v>51</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>14</v>
@@ -4767,10 +4754,10 @@
         <v>98</v>
       </c>
       <c r="M73" s="9" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>97</v>
       </c>
@@ -4790,13 +4777,13 @@
         <v>98</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H74" s="12" t="s">
         <v>51</v>
       </c>
       <c r="I74" s="17" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>14</v>
@@ -4808,10 +4795,10 @@
         <v>98</v>
       </c>
       <c r="M74" s="9" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>97</v>
       </c>
@@ -4837,7 +4824,7 @@
         <v>37</v>
       </c>
       <c r="I75" s="17" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>100</v>
@@ -4849,10 +4836,10 @@
         <v>98</v>
       </c>
       <c r="M75" s="9" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>97</v>
       </c>
@@ -4878,7 +4865,7 @@
         <v>37</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>14</v>
@@ -4890,14 +4877,14 @@
         <v>98</v>
       </c>
       <c r="M76" s="9" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B77" s="20"/>
       <c r="C77" s="20"/>
     </row>
-    <row r="78" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="11" t="s">
         <v>102</v>
       </c>
@@ -4935,10 +4922,10 @@
         <v>103</v>
       </c>
       <c r="M78" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>102</v>
       </c>
@@ -4976,10 +4963,10 @@
         <v>103</v>
       </c>
       <c r="M79" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>102</v>
       </c>
@@ -4990,7 +4977,7 @@
         <v>40992</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E80" t="s">
         <v>15</v>
@@ -5020,7 +5007,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>102</v>
       </c>
@@ -5031,7 +5018,7 @@
         <v>41007</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="E81" t="s">
         <v>15</v>
@@ -5061,7 +5048,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>102</v>
       </c>
@@ -5102,7 +5089,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>102</v>
       </c>
@@ -5143,7 +5130,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>102</v>
       </c>
@@ -5154,7 +5141,7 @@
         <v>44561</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E84" t="s">
         <v>15</v>
@@ -5184,7 +5171,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>102</v>
       </c>
@@ -5195,7 +5182,7 @@
         <v>44561</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
@@ -5225,7 +5212,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>102</v>
       </c>
@@ -5236,7 +5223,7 @@
         <v>44561</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
@@ -5266,7 +5253,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -5277,7 +5264,7 @@
         <v>44561</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -5307,7 +5294,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>102</v>
       </c>
@@ -5318,7 +5305,7 @@
         <v>44561</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -5333,7 +5320,7 @@
         <v>112</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>14</v>
@@ -5348,7 +5335,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>102</v>
       </c>
@@ -5359,7 +5346,7 @@
         <v>44561</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -5371,13 +5358,13 @@
         <v>37</v>
       </c>
       <c r="H89" s="12" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="K89" t="s">
         <v>20</v>
@@ -5389,7 +5376,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>124</v>
       </c>
@@ -5430,7 +5417,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>124</v>
       </c>
@@ -5471,7 +5458,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>124</v>
       </c>
@@ -5512,7 +5499,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>124</v>
       </c>
@@ -5553,7 +5540,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>124</v>
       </c>
@@ -5594,7 +5581,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>124</v>
       </c>
@@ -5635,7 +5622,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>124</v>
       </c>
@@ -5646,7 +5633,7 @@
         <v>44561</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E96" t="s">
         <v>15</v>
@@ -5661,10 +5648,10 @@
         <v>18</v>
       </c>
       <c r="I96" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="K96" t="s">
         <v>20</v>
@@ -5676,7 +5663,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>124</v>
       </c>
@@ -5687,7 +5674,7 @@
         <v>44561</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
@@ -5702,10 +5689,10 @@
         <v>18</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="K97" t="s">
         <v>20</v>
@@ -5717,7 +5704,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>124</v>
       </c>
@@ -5728,7 +5715,7 @@
         <v>44561</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E98" t="s">
         <v>15</v>
@@ -5758,7 +5745,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>124</v>
       </c>
@@ -5769,7 +5756,7 @@
         <v>44561</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E99" t="s">
         <v>15</v>
@@ -5799,12 +5786,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="11"/>
       <c r="B100" s="21"/>
       <c r="C100" s="21"/>
     </row>
-    <row r="101" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>146</v>
       </c>
@@ -5824,7 +5811,7 @@
         <v>147</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H101" s="12" t="s">
         <v>209</v>
@@ -5842,10 +5829,10 @@
         <v>147</v>
       </c>
       <c r="M101" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>146</v>
       </c>
@@ -5865,7 +5852,7 @@
         <v>147</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H102" s="12" t="s">
         <v>209</v>
@@ -5883,10 +5870,10 @@
         <v>147</v>
       </c>
       <c r="M102" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>146</v>
       </c>
@@ -5906,7 +5893,7 @@
         <v>147</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H103" s="12" t="s">
         <v>209</v>
@@ -5924,10 +5911,10 @@
         <v>147</v>
       </c>
       <c r="M103" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>146</v>
       </c>
@@ -5947,7 +5934,7 @@
         <v>147</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H104" s="12" t="s">
         <v>209</v>
@@ -5965,10 +5952,10 @@
         <v>147</v>
       </c>
       <c r="M104" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>146</v>
       </c>
@@ -5988,7 +5975,7 @@
         <v>147</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H105" s="12" t="s">
         <v>209</v>
@@ -6006,10 +5993,10 @@
         <v>147</v>
       </c>
       <c r="M105" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>146</v>
       </c>
@@ -6029,7 +6016,7 @@
         <v>147</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H106" s="12" t="s">
         <v>209</v>
@@ -6047,10 +6034,10 @@
         <v>147</v>
       </c>
       <c r="M106" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>146</v>
       </c>
@@ -6070,7 +6057,7 @@
         <v>147</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H107" s="12" t="s">
         <v>209</v>
@@ -6088,10 +6075,10 @@
         <v>147</v>
       </c>
       <c r="M107" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>146</v>
       </c>
@@ -6111,7 +6098,7 @@
         <v>147</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H108" s="12" t="s">
         <v>209</v>
@@ -6129,10 +6116,10 @@
         <v>147</v>
       </c>
       <c r="M108" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>146</v>
       </c>
@@ -6152,7 +6139,7 @@
         <v>147</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>289</v>
+        <v>208</v>
       </c>
       <c r="H109" s="12" t="s">
         <v>209</v>
@@ -6170,10 +6157,10 @@
         <v>147</v>
       </c>
       <c r="M109" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="110" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>146</v>
       </c>
@@ -6214,7 +6201,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>146</v>
       </c>
@@ -6255,7 +6242,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>146</v>
       </c>
@@ -6296,7 +6283,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>146</v>
       </c>
@@ -6337,7 +6324,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>146</v>
       </c>
@@ -6378,7 +6365,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>146</v>
       </c>
@@ -6419,7 +6406,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>146</v>
       </c>
@@ -6460,7 +6447,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>146</v>
       </c>
@@ -6501,7 +6488,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>146</v>
       </c>
@@ -6542,7 +6529,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>146</v>
       </c>
@@ -6583,7 +6570,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>146</v>
       </c>
@@ -6624,7 +6611,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>146</v>
       </c>
@@ -6665,7 +6652,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>146</v>
       </c>
@@ -6706,7 +6693,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>146</v>
       </c>
@@ -6747,7 +6734,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>146</v>
       </c>
@@ -6788,7 +6775,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>146</v>
       </c>
@@ -6826,10 +6813,10 @@
         <v>147</v>
       </c>
       <c r="M125" s="9" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>146</v>
       </c>
@@ -6840,7 +6827,7 @@
         <v>41027</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E126" t="s">
         <v>15</v>
@@ -6870,19 +6857,19 @@
         <v>151</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B127" s="20"/>
       <c r="C127" s="20"/>
     </row>
-    <row r="128" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>192</v>
       </c>
       <c r="B128" s="20">
         <v>35677</v>
       </c>
-      <c r="C128" s="20" t="s">
-        <v>255</v>
+      <c r="C128" s="20">
+        <v>44926</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>14</v>
@@ -6912,15 +6899,15 @@
         <v>193</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>192</v>
       </c>
       <c r="B129" s="20">
         <v>35677</v>
       </c>
-      <c r="C129" s="20" t="s">
-        <v>255</v>
+      <c r="C129" s="20">
+        <v>44926</v>
       </c>
       <c r="D129" s="4" t="s">
         <v>14</v>
@@ -6950,15 +6937,15 @@
         <v>193</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>192</v>
       </c>
       <c r="B130" s="20">
         <v>35677</v>
       </c>
-      <c r="C130" s="20" t="s">
-        <v>255</v>
+      <c r="C130" s="20">
+        <v>44926</v>
       </c>
       <c r="D130" s="4" t="s">
         <v>14</v>
@@ -6988,15 +6975,15 @@
         <v>193</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>192</v>
       </c>
       <c r="B131" s="20">
         <v>35677</v>
       </c>
-      <c r="C131" s="20" t="s">
-        <v>255</v>
+      <c r="C131" s="20">
+        <v>44926</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>14</v>
@@ -7026,18 +7013,18 @@
         <v>193</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>192</v>
       </c>
       <c r="B132" s="20">
         <v>35677</v>
       </c>
-      <c r="C132" s="20" t="s">
+      <c r="C132" s="20">
+        <v>44926</v>
+      </c>
+      <c r="D132" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="D132" s="4" t="s">
-        <v>256</v>
       </c>
       <c r="E132" t="s">
         <v>15</v>
@@ -7064,21 +7051,21 @@
         <v>193</v>
       </c>
       <c r="M132" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>192</v>
       </c>
       <c r="B133" s="20">
         <v>35677</v>
       </c>
-      <c r="C133" s="20" t="s">
-        <v>255</v>
+      <c r="C133" s="20">
+        <v>44926</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E133" t="s">
         <v>15</v>
@@ -7105,21 +7092,21 @@
         <v>193</v>
       </c>
       <c r="M133" s="9" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>192</v>
       </c>
       <c r="B134" s="20">
         <v>35677</v>
       </c>
-      <c r="C134" s="20" t="s">
-        <v>255</v>
+      <c r="C134" s="20">
+        <v>44926</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E134" t="s">
         <v>15</v>
@@ -7146,21 +7133,21 @@
         <v>193</v>
       </c>
       <c r="M134" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>192</v>
       </c>
       <c r="B135" s="20">
         <v>35677</v>
       </c>
-      <c r="C135" s="20" t="s">
-        <v>255</v>
+      <c r="C135" s="20">
+        <v>44926</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E135" t="s">
         <v>15</v>
@@ -7187,21 +7174,21 @@
         <v>193</v>
       </c>
       <c r="M135" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>192</v>
       </c>
       <c r="B136" s="20">
         <v>35677</v>
       </c>
-      <c r="C136" s="20" t="s">
-        <v>255</v>
+      <c r="C136" s="20">
+        <v>44926</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E136" t="s">
         <v>15</v>
@@ -7228,21 +7215,21 @@
         <v>193</v>
       </c>
       <c r="M136" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>192</v>
       </c>
       <c r="B137" s="20">
         <v>35677</v>
       </c>
-      <c r="C137" s="20" t="s">
-        <v>255</v>
+      <c r="C137" s="20">
+        <v>44926</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E137" t="s">
         <v>15</v>
@@ -7269,21 +7256,21 @@
         <v>193</v>
       </c>
       <c r="M137" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>192</v>
       </c>
       <c r="B138" s="20">
         <v>35677</v>
       </c>
-      <c r="C138" s="20" t="s">
-        <v>255</v>
+      <c r="C138" s="20">
+        <v>44926</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E138" t="s">
         <v>15</v>
@@ -7310,21 +7297,21 @@
         <v>193</v>
       </c>
       <c r="M138" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="139" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>192</v>
       </c>
       <c r="B139" s="20">
         <v>35677</v>
       </c>
-      <c r="C139" s="20" t="s">
-        <v>255</v>
+      <c r="C139" s="20">
+        <v>44926</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E139" t="s">
         <v>15</v>
@@ -7351,21 +7338,21 @@
         <v>193</v>
       </c>
       <c r="M139" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="140" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>192</v>
       </c>
       <c r="B140" s="20">
         <v>35677</v>
       </c>
-      <c r="C140" s="20" t="s">
-        <v>255</v>
+      <c r="C140" s="20">
+        <v>44926</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E140" t="s">
         <v>15</v>
@@ -7392,21 +7379,21 @@
         <v>193</v>
       </c>
       <c r="M140" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>192</v>
       </c>
       <c r="B141" s="20">
         <v>35677</v>
       </c>
-      <c r="C141" s="20" t="s">
-        <v>255</v>
+      <c r="C141" s="20">
+        <v>44926</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E141" t="s">
         <v>15</v>
@@ -7433,14 +7420,14 @@
         <v>193</v>
       </c>
       <c r="M141" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B142" s="20"/>
       <c r="C142" s="20"/>
     </row>
-    <row r="143" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>206</v>
       </c>
@@ -7481,7 +7468,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>206</v>
       </c>
@@ -7522,7 +7509,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>215</v>
       </c>
@@ -7563,7 +7550,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>215</v>
       </c>
@@ -7604,15 +7591,15 @@
         <v>219</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>220</v>
       </c>
       <c r="B147" s="20">
         <v>43009</v>
       </c>
-      <c r="C147" s="20" t="s">
-        <v>268</v>
+      <c r="C147" s="20">
+        <v>44469</v>
       </c>
       <c r="D147" s="4" t="s">
         <v>14</v>
@@ -7642,18 +7629,18 @@
         <v>207</v>
       </c>
       <c r="M147" s="9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="148" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>220</v>
       </c>
       <c r="B148" s="20">
         <v>43009</v>
       </c>
-      <c r="C148" s="20" t="s">
-        <v>269</v>
+      <c r="C148" s="20">
+        <v>43373</v>
       </c>
       <c r="D148" s="4" t="s">
         <v>224</v>
@@ -7686,51 +7673,51 @@
         <v>226</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B149" s="20"/>
       <c r="C149" s="20"/>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B150" s="20"/>
       <c r="C150" s="20"/>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B151" s="20"/>
       <c r="C151" s="20"/>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B152" s="20"/>
       <c r="C152" s="20"/>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B153" s="20"/>
       <c r="C153" s="20"/>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B154" s="20"/>
       <c r="C154" s="20"/>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B155" s="20"/>
       <c r="C155" s="20"/>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B156" s="20"/>
       <c r="C156" s="20"/>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B157" s="20"/>
       <c r="C157" s="20"/>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B158" s="20"/>
       <c r="C158" s="20"/>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B159" s="20"/>
       <c r="C159" s="20"/>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B160" s="20"/>
       <c r="C160" s="20"/>
     </row>
@@ -7770,18 +7757,18 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="105.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="105.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>228</v>
       </c>
@@ -7789,7 +7776,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -7797,7 +7784,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -7805,7 +7792,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>232</v>
       </c>
@@ -7813,7 +7800,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>234</v>
       </c>
@@ -7821,7 +7808,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>111</v>
       </c>
@@ -7829,7 +7816,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -7837,7 +7824,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>238</v>
       </c>
@@ -7845,7 +7832,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>240</v>
       </c>
@@ -7853,7 +7840,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -7861,7 +7848,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -7869,7 +7856,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -7877,7 +7864,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -7885,7 +7872,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -7893,7 +7880,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>247</v>
       </c>
@@ -7901,7 +7888,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>249</v>
       </c>
@@ -7909,7 +7896,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>251</v>
       </c>
@@ -7917,7 +7904,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>253</v>
       </c>
@@ -7932,6 +7919,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="80b53ead-ac38-442a-b597-5a0e2e0802cd">
@@ -7940,15 +7936,6 @@
     <TaxCatchAll xmlns="5ec1cc48-4270-4222-9ed5-54ce9e59d47b" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8189,20 +8176,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B1B5D08-A2EB-4F47-BA81-DA28AA2A09F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66AF2240-620B-4312-9739-CAF731E4A98F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="80b53ead-ac38-442a-b597-5a0e2e0802cd"/>
     <ds:schemaRef ds:uri="5ec1cc48-4270-4222-9ed5-54ce9e59d47b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B1B5D08-A2EB-4F47-BA81-DA28AA2A09F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updated dates on GHG GOSAT2 entries
</commit_message>
<xml_diff>
--- a/EEE2000-metadata_mapping.xlsx
+++ b/EEE2000-metadata_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amw23\Documents\GitHub\cci_data_bridge_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0953501D-529B-4800-8168-775A0D4623FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90B7D6D-A3C1-4747-82F9-25E05EE21E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B9DA58AC-C110-4CBA-A19B-6F37B44EEA38}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B9DA58AC-C110-4CBA-A19B-6F37B44EEA38}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="303">
   <si>
     <t>Dataset 1</t>
   </si>
@@ -207,9 +207,6 @@
 version=2_0</t>
   </si>
   <si>
-    <t>CCI archive on CEDA</t>
-  </si>
-  <si>
     <t>processinglevel=level4,
 sensor_on_satellite=combined_product,
 version=1_1</t>
@@ -333,12 +330,6 @@
     <t>Greenhouse Gases</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/e493802d83c846c8b76f817866fb74cc</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/294b4075ddbc4464bb06742816813bdc</t>
-  </si>
-  <si>
     <t>IsOriginalFormOf</t>
   </si>
   <si>
@@ -360,13 +351,7 @@
     <t>IsPreviousVersionOf</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/9255faeb392f41debf5402caa40dada8</t>
-  </si>
-  <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CO2.TANSO-FTS.GOSAT.OCFP.v7-0-1.r1</t>
-  </si>
-  <si>
-    <t>C3S is a newer version</t>
   </si>
   <si>
     <t>processing_level=level_2,
@@ -375,13 +360,7 @@
 version=2.3.8</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/e61704b00267405082fbd41bb710dd74</t>
-  </si>
-  <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CO2.TANSO-FTS.GOSAT.SRFP.v2-3-8.r1</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/9f002827ba7d48f59019fcfd3577a57e</t>
   </si>
   <si>
     <t>https://doi.org/10.24381/cds.b25419f8</t>
@@ -393,9 +372,6 @@
 version=7.2</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/8f5623a85d2e4b9b8ab5313f65a7c994</t>
-  </si>
-  <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CH4.SCIAMACHY.Envisat.IMAP.v7-2.r1</t>
   </si>
   <si>
@@ -405,9 +381,6 @@
 version=4.0</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/aa09603e91b44f3cb1573c9dd415e8a8</t>
-  </si>
-  <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CH4.SCIAMACHY.Envisat.WFMD.v4-0.r1</t>
   </si>
   <si>
@@ -417,9 +390,6 @@
 version=7.3</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/56f81895cb094bd8a1638aa12d6c7499</t>
-  </si>
-  <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CH4.TANSO-FTS.GOSAT.OCFP.v2-1.r1</t>
   </si>
   <si>
@@ -429,9 +399,6 @@
 version=9.0</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/f9154243fd8744bdaf2a59c39033e659</t>
-  </si>
-  <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CH4.TANSO-FTS.GOSAT.OCPR.v7-0.r1</t>
   </si>
   <si>
@@ -441,9 +408,6 @@
 version=2.3.8</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/46d136149d0a4f1cb8de7efbe8abf4b2</t>
-  </si>
-  <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CH4.TANSO-FTS.GOSAT.SRFP.v2-3-8.r1</t>
   </si>
   <si>
@@ -453,13 +417,7 @@
 version=2.3.9</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/96d5b75ea29946c5aab8214ddbab252b</t>
-  </si>
-  <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CH4.TANSO-FTS.GOSAT.SRPR.v2-3-8.r1</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/9ed2813d2eda4d958e92ab3ce1ab1fe6</t>
   </si>
   <si>
     <t>esacci.GHG.satellite-orbit-frequency.L2.CH4.TANSO-FTS.GOSAT.EMMA.ch4_v1-2.r1</t>
@@ -480,13 +438,7 @@
 sensor_on_satellite=aatsr_on_envisat</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/ab90030e26c54ba495b1cbec51e137e1</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.day.L3C.AER_PRODUCTS.AATSR.Envisat.ADV.2-31.r1</t>
-  </si>
-  <si>
-    <t>C3S is a newer version.</t>
   </si>
   <si>
     <t>time_aggregation=monthly_average,
@@ -504,9 +456,6 @@
 sensor_on_satellite=atsr2_on_ers2</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/302939d341fa4013b6d96d231d6d4f40</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.day.L3C.AER_PRODUCTS.ATSR-2.ERS-2.ADV.2-31.r1</t>
   </si>
   <si>
@@ -525,9 +474,6 @@
 sensor_on_satellite=aatsr_on_envisat</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/c183044b88734442b6d37f5c4f6b0092</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.day.L3C.AER_PRODUCTS.multi-sensor.multi-platform.AATSR-ENVISAT-ENS_DAILY.v2-6.r1</t>
   </si>
   <si>
@@ -546,9 +492,6 @@
 sensor_on_satellite=atsr2_on_ers2</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/bf5eae2a052848aab2abf93d96e7e9aa</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.day.L3C.AER_PRODUCTS.multi-sensor.multi-platform.ATSR2-ENVISAT-ENS_DAILY.v2-6.r1</t>
   </si>
   <si>
@@ -567,9 +510,6 @@
 sensor_on_satellite=aatsr_on_envisat</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/da2b8512312a4f14a928766f7f632d36</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.day.L3C.AER_PRODUCTS.AATSR.Envisat.ORAC.04-01-.r1</t>
   </si>
   <si>
@@ -588,9 +528,6 @@
 sensor_on_satellite=atsr2_on_ers2</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/d2ed0c005761475d92ca444666156c4a</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.day.L3C.AER_PRODUCTS.ATSR-2.ERS-2.ORAC.04-01-.r1</t>
   </si>
   <si>
@@ -609,9 +546,6 @@
 sensor_on_satellite=aatsr_on_envisat</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/d12fc40e4f254ce38303157fa460f01c</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.day.L3C.AER_PRODUCTS.AATSR.Envisat.SU.4-3.r1</t>
   </si>
   <si>
@@ -630,9 +564,6 @@
 sensor_on_satellite=atsr2_on_ers2</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/39909dc233b34118a80dd6fa8a7af553</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.day.L3C.AER_PRODUCTS.ATSR-2.ERS-2.SU.4-3.r1</t>
   </si>
   <si>
@@ -650,9 +581,6 @@
 IsPartOf</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/7fb8fd2761484b1eae4f7df4a3e65f75</t>
-  </si>
-  <si>
     <t>esacci.AEROSOL.5-days.L3C.AEX.GOMOS.Envisat.AERGOM.3-00.r1</t>
   </si>
   <si>
@@ -662,40 +590,7 @@
     <t>Ocean Colour</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/016f577b631a429a8558796a74983154</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.OC_PRODUCTS.multi-sensor.multi-platform.MERGED.5-0.geographic</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/5ab5267b17254152bcdbc055747faa02</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.RRS.multi-sensor.multi-platform.MERGED.5-0.geographic</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/66534da90ed44abebfc1b08adca4f9c3</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.OC_PRODUCTS.multi-sensor.multi-platform.MERGED.5-0.sinusoidal</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/f30495d4425f46c489765a2f84dd6862</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.RRS.multi-sensor.multi-platform.MERGED.5-0.sinusoidal</t>
-  </si>
-  <si>
     <t>https://catalogue.ceda.ac.uk/uuid/e9f82908fd9c48138b31e5cfaa6d692b</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.CHLOR_A.multi-sensor.multi-platform.MERGED.5-0.geographic</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/8154e881452f49c1ba86982ed88b20f0</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.CHLOR_A.multi-sensor.multi-platform.MERGED.5-0.sinusoidal</t>
   </si>
   <si>
     <t>https://doi.org/10.24381/cds.38b9366c</t>
@@ -712,25 +607,13 @@
 IsPreviousVersionOf</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/ff4bfe39b7fe42fc993341d3cebdabb5</t>
-  </si>
-  <si>
     <t>esacci.ICESHEETS.yr.Unspecified.GMB.GRACE-instrument.GRACE.UNSPECIFIED.1-5.greenland_gmb_time_series</t>
   </si>
   <si>
-    <t>C3S product is a combined Greenland and Antarctic product.  C3S data is a later version and in a different format.</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/35ea8189e75e4b6f95e7c86812080ecb</t>
-  </si>
-  <si>
     <t>esacci.ICESHEETS.yr.Unspecified.GMB.GRACE-instrument.GRACE.UNSPECIFIED.1-4.greenland_gmb_time_series</t>
   </si>
   <si>
     <t>https://doi.org/10.24381/cds.056d0df7</t>
-  </si>
-  <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/a7b87a912c494c03b4d2fa5ab8479d1c</t>
   </si>
   <si>
     <t>domain=greenland,
@@ -741,9 +624,6 @@
     <t>esacci.ICESHEETS.yr.Unspecified.SEC.multi-sensor.multi-platform.UNSPECIFIED.1-2.r1</t>
   </si>
   <si>
-    <t>C3S product is a new version of the CCI product</t>
-  </si>
-  <si>
     <t>https://doi.org/10.24381/cds.0b96b838</t>
   </si>
   <si>
@@ -755,17 +635,7 @@
 IsPreviousVersionOf</t>
   </si>
   <si>
-    <t>http://catalogue.ceda.ac.uk/uuid/eaed9fba86c44e9c854dfbdec9d16b99</t>
-  </si>
-  <si>
-    <t>version=1.3,
-period=2017_2018</t>
-  </si>
-  <si>
     <t>esacci.ICESHEETS.unspecified.Unspecified.IV.SAR-C-(Sentinel-1).multi-platform.UNSPECIFIED.1-0.greenland_map_winter_2017_2018</t>
-  </si>
-  <si>
-    <t>C3S product is a newer version of the CCI product</t>
   </si>
   <si>
     <t>Definitions currently taken from DataCite relationType: https://schema.datacite.org/meta/kernel-4.3/doc/DataCite-MetadataKernel_v4.3.pdf</t>
@@ -867,18 +737,6 @@
 version=6_0</t>
   </si>
   <si>
-    <t xml:space="preserve">C3S data is a newer version compared to the CCI data.  It is a subset of the CCI data (CCI data contains multiple time averages). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3S data is a newer version compared to the CCI data.   It is a subset of the CCI data (CCI data contains multiple variables and time averages).  </t>
-  </si>
-  <si>
-    <t>C3S data is a newer version compared to the CCI data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3S data is a newer version compared to the CCI data.  C3S data is a subset of the CCI data (CCI data contains multiple time averages). </t>
-  </si>
-  <si>
     <t>variable=[mass_concentration of chlorophyll_a,remote_sensing_reflectance],
 projection=sinusoidal_grid,
 version=6_0</t>
@@ -892,9 +750,6 @@
     <t>variable=remote_sensing_reflectance,
 projection=sinusoidal_grid,
 version=6_0</t>
-  </si>
-  <si>
-    <t>C3S data is a newer version that the corresponding CCI data</t>
   </si>
   <si>
     <t>CCI product has data up until 2017-2018, while C3S product has data from 2017-2020.   C3S product is a newer version (version depends on date range)</t>
@@ -946,11 +801,6 @@
 version=2.0.0</t>
   </si>
   <si>
-    <t>processing_level=level_2,
-sensor_and_algorithm=tanso2_fts2_srfp,
-version=2.0.1</t>
-  </si>
-  <si>
     <t>IsPartOf,
 IsOriginalFormOf</t>
   </si>
@@ -982,9 +832,6 @@
     <t>CCI data is a subset of the C3S data</t>
   </si>
   <si>
-    <t>CCI data is a subset of the C3S aerosol dataset.  C3S data is a newer version</t>
-  </si>
-  <si>
     <t>https://catalogue.ceda.ac.uk/uuid/a963d9415bb74247830f8704f825aa90</t>
   </si>
   <si>
@@ -1081,15 +928,9 @@
     <t>The C3S MODIS pixel v5_1_1cds subset of the fire burned area (https://doi.org/10.24381/cds.f333cf85) dataset is a reformatted version of the CCI v5.1 pixel data with errata included.  The CCI data extends forward in time.</t>
   </si>
   <si>
-    <t xml:space="preserve">C3S is a newer version.  </t>
-  </si>
-  <si>
     <t>https://catalogue.ceda.ac.uk/uuid/a0782135bcd04d77a1dae4aa71fba47c</t>
   </si>
   <si>
-    <t>esacci.OC.day.L3S.RRS.multi-sensor.multi-platform.MERGED.6-0.geographic</t>
-  </si>
-  <si>
     <t>https://catalogue.ceda.ac.uk/uuid/0875b4675f1e46ebadb526e0b95505c5</t>
   </si>
   <si>
@@ -1103,21 +944,6 @@
   </si>
   <si>
     <t>https://catalogue.ceda.ac.uk/uuid/86d360431f3b4184b89cdd1cd707bb33</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.OC_PRODUCTS.multi-sensor.multi-platform.MERGED.6-0.geographic</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.OC_PRODUCTS.multi-sensor.multi-platform.MERGED.6-0.sinusoidal</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.RRS.multi-sensor.multi-platform.MERGED.6-0.sinusoidal</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.CHLOR_A.multi-sensor.multi-platform.MERGED.6-0.geographic</t>
-  </si>
-  <si>
-    <t>esacci.OC.day.L3S.CHLOR_A.multi-sensor.multi-platform.MERGED.6-0.sinusoidal</t>
   </si>
   <si>
     <t>processinglevel=level_3c,
@@ -1170,12 +996,6 @@
     <t>The C3S data includes and extends the CCI data in time.   The C3S and CCI datasets have different filenames.</t>
   </si>
   <si>
-    <t>IsPartOf, Is NewVersionOf</t>
-  </si>
-  <si>
-    <t>HasPart, IsPreviousVersionOF</t>
-  </si>
-  <si>
     <t xml:space="preserve">The C3S data is a newer version compared to the CCI data.   It is a subset of the CCI data (CCI data contains multiple variables and time averages).  </t>
   </si>
   <si>
@@ -1191,12 +1011,6 @@
     <t>The C3S product is a new version of the CCI product.</t>
   </si>
   <si>
-    <t>IsPartOf, Continues</t>
-  </si>
-  <si>
-    <t>HasPart, IsContinuedBy</t>
-  </si>
-  <si>
     <t>https://catalogue.ceda.ac.uk/uuid/e493802d83c846c8b76f817866fb74cc</t>
   </si>
   <si>
@@ -1297,6 +1111,25 @@
   </si>
   <si>
     <t>The C3S data is a  subset of the CCI data and the files which are provided via C3S are identical in format, specification, and naming convention to the CCI files.   The C3S data only provides only daily average files.  The C3S data continues the CCI data forward in time.</t>
+  </si>
+  <si>
+    <t>CCI Archive on CEDA</t>
+  </si>
+  <si>
+    <t>IsPartOf, 
+IsNewVersionOf</t>
+  </si>
+  <si>
+    <t>IsPartOf,
+ IsNewVersionOf</t>
+  </si>
+  <si>
+    <t>IsPartOf, 
+Continues</t>
+  </si>
+  <si>
+    <t>HasPart, 
+IsContinuedBy</t>
   </si>
 </sst>
 </file>
@@ -1836,28 +1669,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC0B67C-1229-4907-A814-DF79422D0B81}">
   <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="M90" sqref="M90"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="42.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7265625" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" customWidth="1"/>
+    <col min="6" max="6" width="23.7265625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="30.453125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="42.81640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" customWidth="1"/>
+    <col min="12" max="12" width="23.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.1796875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1879,7 +1712,7 @@
       <c r="K1" s="3"/>
       <c r="M1" s="17"/>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1916,7 +1749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1954,10 +1787,10 @@
         <v>16</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1995,14 +1828,14 @@
         <v>16</v>
       </c>
       <c r="M4" s="21" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
     </row>
-    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2040,10 +1873,10 @@
         <v>29</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>33</v>
       </c>
@@ -2081,10 +1914,10 @@
         <v>29</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
@@ -2122,14 +1955,14 @@
         <v>29</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2155,7 +1988,7 @@
         <v>41</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>42</v>
@@ -2167,10 +2000,10 @@
         <v>40</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2196,7 +2029,7 @@
         <v>45</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>259</v>
+        <v>209</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>28</v>
@@ -2208,10 +2041,10 @@
         <v>40</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2237,7 +2070,7 @@
         <v>48</v>
       </c>
       <c r="I12" s="16" t="s">
-        <v>256</v>
+        <v>206</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>28</v>
@@ -2249,10 +2082,10 @@
         <v>40</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2278,22 +2111,22 @@
         <v>45</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>298</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>40</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2304,7 +2137,7 @@
         <v>40543</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
         <v>15</v>
@@ -2319,10 +2152,10 @@
         <v>41</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K14" t="s">
         <v>19</v>
@@ -2331,10 +2164,10 @@
         <v>40</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2345,7 +2178,7 @@
         <v>35074</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -2360,7 +2193,7 @@
         <v>44</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>28</v>
@@ -2372,10 +2205,10 @@
         <v>40</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2386,7 +2219,7 @@
         <v>37794</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
@@ -2401,7 +2234,7 @@
         <v>44</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>28</v>
@@ -2413,10 +2246,10 @@
         <v>40</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2427,7 +2260,7 @@
         <v>41007</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
@@ -2442,7 +2275,7 @@
         <v>44</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>28</v>
@@ -2454,10 +2287,10 @@
         <v>40</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2468,7 +2301,7 @@
         <v>35074</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
@@ -2483,22 +2316,22 @@
         <v>44</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="J18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K18" t="s">
-        <v>50</v>
+        <v>298</v>
       </c>
       <c r="L18" s="6" t="s">
         <v>40</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2509,7 +2342,7 @@
         <v>37794</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
@@ -2524,22 +2357,22 @@
         <v>44</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="J19" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K19" t="s">
-        <v>50</v>
+        <v>298</v>
       </c>
       <c r="L19" s="6" t="s">
         <v>40</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2550,7 +2383,7 @@
         <v>41007</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
         <v>15</v>
@@ -2565,22 +2398,22 @@
         <v>44</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>28</v>
       </c>
       <c r="K20" t="s">
-        <v>50</v>
+        <v>298</v>
       </c>
       <c r="L20" s="6" t="s">
         <v>40</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2591,7 +2424,7 @@
         <v>31094</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
         <v>15</v>
@@ -2606,7 +2439,7 @@
         <v>44</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J21" s="4" t="s">
         <v>14</v>
@@ -2618,10 +2451,10 @@
         <v>40</v>
       </c>
       <c r="M21" s="8" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2632,7 +2465,7 @@
         <v>32454</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" t="s">
         <v>15</v>
@@ -2647,7 +2480,7 @@
         <v>44</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J22" s="4" t="s">
         <v>14</v>
@@ -2659,10 +2492,10 @@
         <v>40</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2673,7 +2506,7 @@
         <v>34590</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
@@ -2688,7 +2521,7 @@
         <v>44</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>14</v>
@@ -2700,10 +2533,10 @@
         <v>40</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -2714,7 +2547,7 @@
         <v>36143</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
@@ -2729,7 +2562,7 @@
         <v>44</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J24" s="4" t="s">
         <v>14</v>
@@ -2741,10 +2574,10 @@
         <v>40</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -2755,7 +2588,7 @@
         <v>36525</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
@@ -2770,7 +2603,7 @@
         <v>44</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>14</v>
@@ -2782,10 +2615,10 @@
         <v>40</v>
       </c>
       <c r="M25" s="8" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2796,7 +2629,7 @@
         <v>40178</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" t="s">
         <v>15</v>
@@ -2811,7 +2644,7 @@
         <v>44</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>14</v>
@@ -2823,10 +2656,10 @@
         <v>40</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2837,7 +2670,7 @@
         <v>39082</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E27" t="s">
         <v>15</v>
@@ -2852,7 +2685,7 @@
         <v>44</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>14</v>
@@ -2864,10 +2697,10 @@
         <v>40</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -2878,7 +2711,7 @@
         <v>40178</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
@@ -2893,7 +2726,7 @@
         <v>44</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J28" s="4" t="s">
         <v>14</v>
@@ -2905,10 +2738,10 @@
         <v>40</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2919,7 +2752,7 @@
         <v>40178</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
@@ -2934,7 +2767,7 @@
         <v>44</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>14</v>
@@ -2946,10 +2779,10 @@
         <v>40</v>
       </c>
       <c r="M29" s="8" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -2960,7 +2793,7 @@
         <v>43465</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -2975,7 +2808,7 @@
         <v>47</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>14</v>
@@ -2987,10 +2820,10 @@
         <v>40</v>
       </c>
       <c r="M30" s="8" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -3001,7 +2834,7 @@
         <v>44469</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
@@ -3016,7 +2849,7 @@
         <v>48</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J31" s="4" t="s">
         <v>14</v>
@@ -3028,10 +2861,10 @@
         <v>40</v>
       </c>
       <c r="M31" s="8" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -3042,7 +2875,7 @@
         <v>44926</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>300</v>
+        <v>243</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
@@ -3057,7 +2890,7 @@
         <v>24</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J32" s="4" t="s">
         <v>14</v>
@@ -3069,16 +2902,16 @@
         <v>40</v>
       </c>
       <c r="M32" s="8" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
     </row>
-    <row r="34" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="19">
         <v>36892</v>
@@ -3087,13 +2920,13 @@
         <v>43830</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E34" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>17</v>
@@ -3102,24 +2935,24 @@
         <v>32</v>
       </c>
       <c r="I34" s="16" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K34" t="s">
         <v>19</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" s="19">
         <v>36892</v>
@@ -3128,13 +2961,13 @@
         <v>43830</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E35" t="s">
         <v>15</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>17</v>
@@ -3143,7 +2976,7 @@
         <v>32</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="J35" s="4" t="s">
         <v>14</v>
@@ -3152,19 +2985,19 @@
         <v>19</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M35" s="8" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
     </row>
-    <row r="37" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" s="19">
         <v>37629</v>
@@ -3173,39 +3006,39 @@
         <v>40992</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>237</v>
+        <v>189</v>
       </c>
       <c r="E37" t="s">
         <v>15</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>325</v>
+        <v>264</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K37" t="s">
         <v>19</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M37" s="8" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38" s="19">
         <v>37530</v>
@@ -3214,39 +3047,39 @@
         <v>41007</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>238</v>
+        <v>190</v>
       </c>
       <c r="E38" t="s">
         <v>15</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>326</v>
+        <v>265</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K38" t="s">
         <v>19</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" s="19">
         <v>39921</v>
@@ -3255,39 +3088,39 @@
         <v>44561</v>
       </c>
       <c r="D39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I39" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="J39" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>327</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="K39" t="s">
         <v>19</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" s="19">
         <v>39904</v>
@@ -3296,13 +3129,13 @@
         <v>44011</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>32</v>
@@ -3311,24 +3144,24 @@
         <v>17</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>328</v>
+        <v>267</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="K40" t="s">
         <v>19</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M40" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="19">
         <v>37629</v>
@@ -3337,22 +3170,22 @@
         <v>44561</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>239</v>
+        <v>191</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H41" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>329</v>
+        <v>268</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>14</v>
@@ -3361,15 +3194,15 @@
         <v>19</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M41" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" s="19">
         <v>37622</v>
@@ -3378,22 +3211,22 @@
         <v>44561</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="E42" t="s">
         <v>15</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H42" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>263</v>
+        <v>213</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>14</v>
@@ -3402,15 +3235,15 @@
         <v>19</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M42" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="19">
         <v>43501</v>
@@ -3419,39 +3252,39 @@
         <v>44561</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>243</v>
+        <v>195</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>241</v>
+        <v>193</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>242</v>
+        <v>194</v>
       </c>
       <c r="K43" t="s">
         <v>19</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B44" s="19">
         <v>37629</v>
@@ -3460,39 +3293,39 @@
         <v>41007</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
         <v>15</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>330</v>
+        <v>269</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="K44" t="s">
         <v>19</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B45" s="19">
         <v>37530</v>
@@ -3501,39 +3334,39 @@
         <v>40908</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
         <v>15</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>331</v>
+        <v>270</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="K45" t="s">
         <v>19</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B46" s="19">
         <v>39921</v>
@@ -3542,39 +3375,39 @@
         <v>44561</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="E46" t="s">
         <v>15</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>332</v>
+        <v>271</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="K46" t="s">
         <v>19</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M46" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B47" s="19">
         <v>39926</v>
@@ -3583,39 +3416,39 @@
         <v>44561</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E47" t="s">
         <v>15</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>333</v>
+        <v>272</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="K47" t="s">
         <v>19</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B48" s="19">
         <v>39904</v>
@@ -3624,13 +3457,13 @@
         <v>44011</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E48" t="s">
         <v>15</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>32</v>
@@ -3639,24 +3472,24 @@
         <v>17</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>334</v>
+        <v>273</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="K48" t="s">
         <v>19</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M48" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B49" s="19">
         <v>39904</v>
@@ -3665,13 +3498,13 @@
         <v>44011</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G49" s="8" t="s">
         <v>32</v>
@@ -3680,39 +3513,39 @@
         <v>17</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>335</v>
+        <v>274</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="K49" t="s">
         <v>19</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B50" s="19">
-        <v>39849</v>
+        <v>43501</v>
       </c>
       <c r="C50" s="19">
         <v>44561</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="E50" t="s">
         <v>15</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>32</v>
@@ -3721,39 +3554,39 @@
         <v>17</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>247</v>
+        <v>198</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="K50" t="s">
         <v>19</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M50" s="8" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B51" s="19">
-        <v>39849</v>
+        <v>43501</v>
       </c>
       <c r="C51" s="19">
         <v>44561</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="E51" t="s">
         <v>15</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G51" s="8" t="s">
         <v>32</v>
@@ -3762,24 +3595,24 @@
         <v>17</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>249</v>
+        <v>200</v>
       </c>
       <c r="K51" t="s">
         <v>19</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M51" s="8" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B52" s="19">
         <v>37627</v>
@@ -3788,39 +3621,39 @@
         <v>44561</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>251</v>
+        <v>202</v>
       </c>
       <c r="E52" t="s">
         <v>15</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>336</v>
+        <v>275</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="K52" t="s">
         <v>19</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M52" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B53" s="19">
         <v>37622</v>
@@ -3829,22 +3662,22 @@
         <v>44561</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>252</v>
+        <v>203</v>
       </c>
       <c r="E53" t="s">
         <v>15</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>14</v>
@@ -3853,20 +3686,20 @@
         <v>19</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M53" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="10"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
     </row>
-    <row r="55" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B55" s="19">
         <v>37469</v>
@@ -3875,39 +3708,39 @@
         <v>41007</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="E55" t="s">
         <v>15</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>337</v>
+        <v>276</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="K55" t="s">
         <v>19</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M55" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B56" s="19">
         <v>37470</v>
@@ -3916,39 +3749,39 @@
         <v>40908</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="E56" t="s">
         <v>15</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>337</v>
+        <v>276</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="K56" t="s">
         <v>19</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M56" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B57" s="19">
         <v>34851</v>
@@ -3957,39 +3790,39 @@
         <v>37729</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="E57" t="s">
         <v>15</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>338</v>
+        <v>277</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="K57" t="s">
         <v>19</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M57" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B58" s="19">
         <v>34851</v>
@@ -3998,39 +3831,39 @@
         <v>37729</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E58" t="s">
         <v>15</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H58" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>338</v>
+        <v>277</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="K58" t="s">
         <v>19</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M58" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B59" s="19">
         <v>37396</v>
@@ -4039,39 +3872,39 @@
         <v>41007</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E59" t="s">
         <v>15</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H59" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>339</v>
+        <v>278</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="K59" t="s">
         <v>19</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M59" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B60" s="19">
         <v>37396</v>
@@ -4080,39 +3913,39 @@
         <v>41007</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="E60" t="s">
         <v>15</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>339</v>
+        <v>278</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="K60" t="s">
         <v>19</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M60" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B61" s="19">
         <v>34851</v>
@@ -4121,39 +3954,39 @@
         <v>37794</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="E61" t="s">
         <v>15</v>
       </c>
       <c r="F61" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H61" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="J61" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G61" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="H61" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="K61" t="s">
         <v>19</v>
       </c>
       <c r="L61" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M61" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B62" s="19">
         <v>34851</v>
@@ -4162,39 +3995,39 @@
         <v>37794</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="E62" t="s">
         <v>15</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H62" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>340</v>
+        <v>279</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="K62" t="s">
         <v>19</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M62" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B63" s="19">
         <v>37396</v>
@@ -4203,39 +4036,39 @@
         <v>41007</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="E63" t="s">
         <v>15</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>341</v>
+        <v>280</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="K63" t="s">
         <v>19</v>
       </c>
       <c r="L63" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M63" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B64" s="19">
         <v>37396</v>
@@ -4244,39 +4077,39 @@
         <v>41007</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="E64" t="s">
         <v>15</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H64" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>341</v>
+        <v>280</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="K64" t="s">
         <v>19</v>
       </c>
       <c r="L64" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M64" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B65" s="19">
         <v>34851</v>
@@ -4285,39 +4118,39 @@
         <v>37835</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="E65" t="s">
         <v>15</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H65" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>342</v>
+        <v>281</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="K65" t="s">
         <v>19</v>
       </c>
       <c r="L65" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M65" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B66" s="19">
         <v>34851</v>
@@ -4326,39 +4159,39 @@
         <v>37835</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E66" t="s">
         <v>15</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>342</v>
+        <v>281</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="K66" t="s">
         <v>19</v>
       </c>
       <c r="L66" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B67" s="19">
         <v>37396</v>
@@ -4367,39 +4200,39 @@
         <v>41007</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="E67" t="s">
         <v>15</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H67" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>343</v>
+        <v>282</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="K67" t="s">
         <v>19</v>
       </c>
       <c r="L67" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M67" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B68" s="19">
         <v>37396</v>
@@ -4408,39 +4241,39 @@
         <v>41007</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="E68" t="s">
         <v>15</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H68" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>343</v>
+        <v>282</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="K68" t="s">
         <v>19</v>
       </c>
       <c r="L68" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M68" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B69" s="19">
         <v>34851</v>
@@ -4449,39 +4282,39 @@
         <v>37794</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="E69" t="s">
         <v>15</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H69" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>344</v>
+        <v>283</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>155</v>
+        <v>132</v>
       </c>
       <c r="K69" t="s">
         <v>19</v>
       </c>
       <c r="L69" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M69" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B70" s="19">
         <v>34851</v>
@@ -4490,22 +4323,22 @@
         <v>37794</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="E70" t="s">
         <v>15</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>344</v>
+        <v>283</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>14</v>
@@ -4514,15 +4347,15 @@
         <v>19</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M70" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B71" s="19">
         <v>37347</v>
@@ -4531,43 +4364,43 @@
         <v>41027</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>236</v>
+        <v>188</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H71" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>345</v>
+        <v>284</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
       <c r="K71" t="s">
         <v>19</v>
       </c>
       <c r="L71" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="M71" s="8" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
     </row>
-    <row r="73" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B73" s="19">
         <v>35677</v>
@@ -4576,36 +4409,39 @@
         <v>45016</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="E73" t="s">
         <v>15</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G73" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="H73" s="12" t="s">
-        <v>317</v>
+        <v>138</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H73" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>346</v>
+        <v>285</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K73" t="s">
         <v>19</v>
       </c>
       <c r="L73" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M73" s="8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B74" s="19">
         <v>35677</v>
@@ -4614,22 +4450,22 @@
         <v>45016</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="E74" t="s">
         <v>15</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G74" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="H74" s="12" t="s">
-        <v>317</v>
+        <v>138</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="H74" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>14</v>
@@ -4638,15 +4474,15 @@
         <v>19</v>
       </c>
       <c r="L74" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M74" s="8" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B75" s="19">
         <v>35677</v>
@@ -4655,22 +4491,22 @@
         <v>45016</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
       <c r="E75" t="s">
         <v>15</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="H75" s="12" t="s">
-        <v>317</v>
+        <v>138</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H75" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>347</v>
+        <v>286</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>14</v>
@@ -4679,15 +4515,15 @@
         <v>19</v>
       </c>
       <c r="L75" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M75" s="8" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B76" s="19">
         <v>35677</v>
@@ -4696,36 +4532,39 @@
         <v>45016</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="E76" t="s">
         <v>15</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G76" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="H76" s="12" t="s">
-        <v>317</v>
+        <v>138</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H76" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>348</v>
+        <v>287</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K76" t="s">
         <v>19</v>
       </c>
       <c r="L76" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M76" s="8" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B77" s="19">
         <v>35677</v>
@@ -4734,22 +4573,22 @@
         <v>45016</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>232</v>
+        <v>185</v>
       </c>
       <c r="E77" t="s">
         <v>15</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G77" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="H77" s="12" t="s">
-        <v>317</v>
+        <v>138</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H77" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>349</v>
+        <v>288</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>14</v>
@@ -4758,15 +4597,15 @@
         <v>19</v>
       </c>
       <c r="L77" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M77" s="8" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B78" s="19">
         <v>35677</v>
@@ -4775,22 +4614,22 @@
         <v>45016</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>233</v>
+        <v>186</v>
       </c>
       <c r="E78" t="s">
         <v>15</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G78" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="H78" s="12" t="s">
-        <v>317</v>
+        <v>138</v>
+      </c>
+      <c r="G78" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="H78" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>350</v>
+        <v>289</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>14</v>
@@ -4799,19 +4638,22 @@
         <v>19</v>
       </c>
       <c r="L78" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M78" s="8" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
-    </row>
-    <row r="80" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="H79" s="11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B80" s="19">
         <v>37347</v>
@@ -4826,33 +4668,33 @@
         <v>15</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>351</v>
+        <v>290</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="K80" t="s">
         <v>19</v>
       </c>
       <c r="L80" s="6" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="B81" s="19">
         <v>37347</v>
@@ -4867,33 +4709,33 @@
         <v>15</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>352</v>
+        <v>291</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="K81" t="s">
         <v>19</v>
       </c>
       <c r="L81" s="6" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="M81" s="8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="B82" s="19">
         <v>33604</v>
@@ -4902,39 +4744,39 @@
         <v>44013</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H82" s="12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>353</v>
+        <v>292</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="K82" t="s">
         <v>19</v>
       </c>
       <c r="L82" s="6" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="M82" s="8" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="116" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="B83" s="19">
         <v>43009</v>
@@ -4949,37 +4791,37 @@
         <v>15</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>190</v>
+        <v>150</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>354</v>
+        <v>293</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="K83" t="s">
         <v>19</v>
       </c>
       <c r="L83" s="6" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="M83" s="8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B84" s="19"/>
       <c r="C84" s="19"/>
     </row>
-    <row r="85" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B85" s="19">
         <v>35677</v>
@@ -4988,36 +4830,39 @@
         <v>45016</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="E85" t="s">
         <v>15</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="G85" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="H85" s="12" t="s">
-        <v>324</v>
+        <v>138</v>
+      </c>
+      <c r="G85" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>302</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>290</v>
+        <v>238</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K85" t="s">
         <v>19</v>
       </c>
       <c r="L85" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M85" s="8" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B86" s="19">
         <v>35677</v>
@@ -5026,13 +4871,13 @@
         <v>45016</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="E86" t="s">
         <v>15</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="G86" s="9" t="s">
         <v>45</v>
@@ -5041,7 +4886,7 @@
         <v>44</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>293</v>
+        <v>241</v>
       </c>
       <c r="J86" s="4" t="s">
         <v>14</v>
@@ -5050,15 +4895,15 @@
         <v>19</v>
       </c>
       <c r="L86" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M86" s="8" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B87" s="19">
         <v>35677</v>
@@ -5067,13 +4912,13 @@
         <v>45016</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>226</v>
+        <v>183</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="G87" s="9" t="s">
         <v>45</v>
@@ -5082,7 +4927,7 @@
         <v>44</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>14</v>
@@ -5091,15 +4936,15 @@
         <v>19</v>
       </c>
       <c r="L87" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M87" s="8" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B88" s="19">
         <v>35677</v>
@@ -5108,13 +4953,13 @@
         <v>45016</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="G88" s="9" t="s">
         <v>45</v>
@@ -5123,21 +4968,24 @@
         <v>44</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>294</v>
+        <v>242</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="K88" t="s">
         <v>19</v>
       </c>
       <c r="L88" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M88" s="8" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B89" s="19">
         <v>35677</v>
@@ -5146,13 +4994,13 @@
         <v>45016</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>232</v>
+        <v>185</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="G89" s="9" t="s">
         <v>45</v>
@@ -5161,7 +5009,7 @@
         <v>44</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>291</v>
+        <v>239</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>14</v>
@@ -5170,15 +5018,15 @@
         <v>19</v>
       </c>
       <c r="L89" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M89" s="8" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="B90" s="19">
         <v>35677</v>
@@ -5187,13 +5035,13 @@
         <v>45016</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>233</v>
+        <v>186</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="G90" s="9" t="s">
         <v>45</v>
@@ -5202,7 +5050,7 @@
         <v>44</v>
       </c>
       <c r="I90" s="16" t="s">
-        <v>292</v>
+        <v>240</v>
       </c>
       <c r="J90" s="4" t="s">
         <v>14</v>
@@ -5211,10 +5059,10 @@
         <v>19</v>
       </c>
       <c r="L90" s="6" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="M90" s="8" t="s">
-        <v>356</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -5249,159 +5097,159 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="105.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="105.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>218</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>222</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -5411,6 +5259,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="80b53ead-ac38-442a-b597-5a0e2e0802cd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="5ec1cc48-4270-4222-9ed5-54ce9e59d47b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010050398B8EA2737947995C227484EA02C8" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc9a2575e6c24a964f45b6e1606b04fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="80b53ead-ac38-442a-b597-5a0e2e0802cd" xmlns:ns3="5ec1cc48-4270-4222-9ed5-54ce9e59d47b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="662112485a0135ca1785eae0908ad389" ns2:_="" ns3:_="">
     <xsd:import namespace="80b53ead-ac38-442a-b597-5a0e2e0802cd"/>
@@ -5647,27 +5515,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="80b53ead-ac38-442a-b597-5a0e2e0802cd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="5ec1cc48-4270-4222-9ed5-54ce9e59d47b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B1B5D08-A2EB-4F47-BA81-DA28AA2A09F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66AF2240-620B-4312-9739-CAF731E4A98F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="80b53ead-ac38-442a-b597-5a0e2e0802cd"/>
+    <ds:schemaRef ds:uri="5ec1cc48-4270-4222-9ed5-54ce9e59d47b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72DD370E-74FD-4D33-B5A7-49A7FE6518F7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5684,23 +5551,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66AF2240-620B-4312-9739-CAF731E4A98F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="80b53ead-ac38-442a-b597-5a0e2e0802cd"/>
-    <ds:schemaRef ds:uri="5ec1cc48-4270-4222-9ed5-54ce9e59d47b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B1B5D08-A2EB-4F47-BA81-DA28AA2A09F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update including remaining ECV's
Updated the mapping to include remaining CCI ECV's and updates to some existing ECV's.
</commit_message>
<xml_diff>
--- a/EEE2000-metadata_mapping.xlsx
+++ b/EEE2000-metadata_mapping.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amw23\Documents\GitHub\cci_data_bridge_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D274DDD-31C6-4697-87AE-9DF39079ED88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E758D98E-D313-43BF-A8A4-6EE68D73BA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B9DA58AC-C110-4CBA-A19B-6F37B44EEA38}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B9DA58AC-C110-4CBA-A19B-6F37B44EEA38}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="2" r:id="rId1"/>
     <sheet name="Relationship definitions" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapping!$L$1:$L$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Mapping!$L$1:$L$92</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="450">
   <si>
     <t>Dataset 1</t>
   </si>
@@ -1130,6 +1130,605 @@
   </si>
   <si>
     <t>esacci.ICESHEETS.yr.Unspecified.SEC.multi-sensor.multi-platform.UNSPECIFIED.1-2.r2</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.553f1387</t>
+  </si>
+  <si>
+    <t>Glaciers</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/5daf1ff8dd2941a18bb4120ceea95721</t>
+  </si>
+  <si>
+    <t>variable=glacier_area,
+product_type=['gridded','hypsometry','vector']
+version=6_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The C3S gridded data is a newer version (v6.0) of the CCI dataset, provided in netCDF format.   The wider C3S product also makes vector and hypsometry data available.   </t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.4c328c78</t>
+  </si>
+  <si>
+    <t>variable=monthly_mean,
+version=vDT2021</t>
+  </si>
+  <si>
+    <t>Sea Level</t>
+  </si>
+  <si>
+    <t>IsNewVersionOf,
+Continues</t>
+  </si>
+  <si>
+    <t>IsPreviousVersionOf,
+IsContinuedBy</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/142052b9dc754f6da47a631e35ec4609</t>
+  </si>
+  <si>
+    <t>The C3S data is a newer version of the CCI dataset and continues the data forward in time.   The C3S data also contains additional variables.</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/e1dfd0ee655944b8a82ce0479c518747</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/36dae49c76f845a18062fa96599be719</t>
+  </si>
+  <si>
+    <t>HasPart,
+IsNewVersionOf,
+IsVariantFormOf</t>
+  </si>
+  <si>
+    <t>IsPartOf,
+IsPreviousVersionOf,
+IsVariantFormOf</t>
+  </si>
+  <si>
+    <t>The C3S product is a combined Greenland and Antarctic product .  The C3S data is a later version that then CCI and in a different format and has been gridded over the major drainage basins.  The CCI dataset is an earlier version and has been gridded on a 50x50km grid.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.d36187ac</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.5714c668</t>
+  </si>
+  <si>
+    <t>version=4.5.1</t>
+  </si>
+  <si>
+    <t>Lakes</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/7fc9df8070d34cacab8092e45ef276f1</t>
+  </si>
+  <si>
+    <t>HasPart,
+IsVariantFormOf,
+Continues</t>
+  </si>
+  <si>
+    <t>IsPartOf,
+IsVariantFormOf,
+IsContinuedBy</t>
+  </si>
+  <si>
+    <t>version=4.5.2</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/7fc9df8070d34cacab8092e45ef276f2</t>
+  </si>
+  <si>
+    <t>The C3S LSWT dataset up to the end of 2020 is a brokered form of a subset of the variables in the CCI dataset. Data is provided in different formats.  The CCI data continues the dataset to the end of 2022, whilst the C3S dataset is continued by the separate v4.5.1 Interim-CDR in C3S.</t>
+  </si>
+  <si>
+    <t>The C3S LSWT v4.5.2 data from 2021 onwards is an Interim-CDR extension of the CCI dataset.   The CDR produced under CCI overlaps in the period up to the end of 2022, while the C3S dataset extends this.</t>
+  </si>
+  <si>
+    <t>IsPartOf,
+IsPreviousVersionOf,
+Continues</t>
+  </si>
+  <si>
+    <t>HasPart,
+IsNewVersionOf,
+IsContinuedBy</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/7fc9df8070d34cacab8092e45ef276f3</t>
+  </si>
+  <si>
+    <t>31/04/2023</t>
+  </si>
+  <si>
+    <t>IsPartOf,
+Continues</t>
+  </si>
+  <si>
+    <t>HasPart,
+IsContinuedBy</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.6679a99a</t>
+  </si>
+  <si>
+    <t>version=3_0
+cdr_type=cdr,
+satellite=envisat</t>
+  </si>
+  <si>
+    <t>version=3_0
+cdr_type=cdr,
+satellite=cryosat_2</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/45b5b1e556da448089e2b57452f277f5</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/83b11005a3d7472eb57df4f90933c462</t>
+  </si>
+  <si>
+    <t>Sea Ice</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.29c46d83</t>
+  </si>
+  <si>
+    <t>version=v3,
+sensor=amsr,
+origin=EUMETSAT OSI SAF</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/f17f146a31b14dfd960cde0874236ee5</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/f17f146a31b14dfd960cde0874236ee6</t>
+  </si>
+  <si>
+    <t>The C3S data is a brokered version of a EUMETSAT SAF dataset, both of which are newer versions of the CCI product.</t>
+  </si>
+  <si>
+    <t>The C3S data is a brokered version of the EUMETSAT OSI SAF dataset.</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/eade27004395466aaa006135e1b2ad1a</t>
+  </si>
+  <si>
+    <t>The CCI dataset is an enhanced-resolution version of the EUMETSAT OSI-SAF CDR which is brokered on C3S</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.29c46d86</t>
+  </si>
+  <si>
+    <t>version=v3,
+sensor=ssmis
+origin=EUMETSAT OSI SAF,
+temporal_aggregation=daily
+cdr_type=cdr</t>
+  </si>
+  <si>
+    <t>OSI SAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The CCI dataset is an enhanced-resolution version of the EUMETSAT OSI-SAF CDR </t>
+  </si>
+  <si>
+    <t>http://doi.org/10.15770/EUM_SAF_OSI_0015</t>
+  </si>
+  <si>
+    <t>http://doi.org/10.15770/EUM_SAF_OSI_0013</t>
+  </si>
+  <si>
+    <t>OSI-458</t>
+  </si>
+  <si>
+    <t>The EUMETSAT OSI SAF dataset is a newer version of the CCI product.</t>
+  </si>
+  <si>
+    <t>version=3_0
+cdr_type=icdr,
+satellite=cryosat_2</t>
+  </si>
+  <si>
+    <t>OSI-450-a</t>
+  </si>
+  <si>
+    <t>IsVariantFormOf,
+Continues</t>
+  </si>
+  <si>
+    <t>IsVariantFormOf,
+IsContinuedBy</t>
+  </si>
+  <si>
+    <t>The C3S sea ice thickness CDR is the CCI SIT CDR v3.0 with a slightly different file format</t>
+  </si>
+  <si>
+    <t>The C3S ICDR (Interim-CDR) extends the CDR dataset forward in time to present with a delay of around 1 month.  The file format is slightly different to the CCI data.</t>
+  </si>
+  <si>
+    <t>CM SAF</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/fab3d1d8abce46f6a53270b0b48a9312</t>
+  </si>
+  <si>
+    <t>Water Vapour</t>
+  </si>
+  <si>
+    <t>The CCI dataset record links directly to the CM SAF dataset.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.8e0e4724</t>
+  </si>
+  <si>
+    <t>C3S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+IsIdenticalTo</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.5676/EUM_SAF_CM/COMBI/V001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The C3S data is identical to the CM-SAF dataset </t>
+  </si>
+  <si>
+    <t>version=near_infrared_hoaps_combined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The C3S data is identical to the CCI dataset which links directly to the CM SAF dataset </t>
+  </si>
+  <si>
+    <t>Soil Moisture</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf65</t>
+  </si>
+  <si>
+    <t>type_of_sensor=active,
+variable=surface_soil_moisture,
+time_aggregation=day_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.d7782f18</t>
+  </si>
+  <si>
+    <t>type_of_sensor=active,
+variable=surface_soil_moisture,
+time_aggregation=day_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>IsPreviousVersionOf,
+IsVariantFormOf</t>
+  </si>
+  <si>
+    <t>IsNewVersionOf,
+IsVariantFormOf</t>
+  </si>
+  <si>
+    <t>IsPreviousVersionOf,
+IsVariantFormOf,
+Continues</t>
+  </si>
+  <si>
+    <t>IsNewVersionOf,
+IsVariantFormOf,
+IsContinuedBy</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf66</t>
+  </si>
+  <si>
+    <t>The C3S CDR dataset corresonds to an earlier version of the CCI dataset and has a different format</t>
+  </si>
+  <si>
+    <t>The C3S ICDR dataset continues the CDR dataset forward in time to the present.  It is based on an earlier version that the current CCI dataset and has a different format.</t>
+  </si>
+  <si>
+    <t>type_of_sensor=active,
+variable=surface_soil_moisture,
+time_aggregation=10_day_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=active,
+variable=surface_soil_moisture,
+time_aggregation=10_day_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=active,
+variable=surface_soil_moisture,
+time_aggregation=month_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=active,
+variable=surface_soil_moisture,
+time_aggregation=month_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>IsSupplementTo,
+IsVariantFormOf,
+IsPreviousVersionOf</t>
+  </si>
+  <si>
+    <t>IsSupplementedBy,
+IsVariantFormOf,
+IsPreviousVersionOf</t>
+  </si>
+  <si>
+    <t>IsSupplementTo,
+IsVariantFormOf,
+IsPreviousVersionOf,
+Continues</t>
+  </si>
+  <si>
+    <t>IsSupplementedBy,
+IsVariantFormOf,
+IsPreviousVersionOf,
+Continues</t>
+  </si>
+  <si>
+    <t>The C3S CDR dataset has a 10-day averaged version of the data.  This corresponds to an earlier version of the algorithm used for the v8.1 CCI dataset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The C3S ICDR dataset has a 10-day averaged version of the data continuing forward to present.  This corresponds to an earlier version of the algorithm used for the v8.1 CCI dataset. </t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf67</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf68</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf69</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf70</t>
+  </si>
+  <si>
+    <t>The C3S CDR dataset has a monthly averaged version of the data.  This corresponds to an earlier version of the algorithm used for the v8.1 CCI dataset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The C3S ICDR dataset has a monthly averaged version of the data continuing forward to present.  This corresponds to an earlier version of the algorithm used for the v8.1 CCI dataset. </t>
+  </si>
+  <si>
+    <t>type_of_sensor=passive,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=10_day_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=passive,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=month_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=passive,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=month_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=passive,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=day_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=passive,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=day_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=passive,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=10_day_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf71</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf72</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf73</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf74</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf75</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b0f5fc3a10cf4806ab57326edd8daf76</t>
+  </si>
+  <si>
+    <t>type_of_sensor=combined_passive_and_active,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=day_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=combined_passive_and_active,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=day_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=combined_passive_and_active,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=10_day_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=combined_passive_and_active,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=10_day_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=combined_passive_and_active,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=month_average,
+type_of_record=cdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>type_of_sensor=combined_passive_and_active,
+variable=volumetric_surface_soil_moisture,
+time_aggregation=month_average,
+type_of_record=icdr,
+version='v202212'</t>
+  </si>
+  <si>
+    <t>version=version_4_0</t>
+  </si>
+  <si>
+    <t>The version 4 Lakes C3S dataset is based on the CCI algorithms.  The CCI dataset includes more than 500 target lakes defined in the CCI project, whilst the C3S dataset contains only operational lakes (where a measurement is added each time the lake is observed by a satellite with altimetry sensors.)   The C3S dataset includes some lakes that are not part of the CCI target lakes.  This version contains 229 lakes in total.   The C3S dataset consists of one file per lake per lake water product, whilst the CCI data is provided as daily files with all lakes included and alongside other lake variables.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.4ebfe4eb</t>
+  </si>
+  <si>
+    <t>processing_level=level_3,
+variable=atmospheric_mole_content_of_ozone,
+vertical_aggregation=total_column,
+sensor=merged_uv,
+version=v2000</t>
+  </si>
+  <si>
+    <t>Ozone</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/0d2260ad4e2c42b6b14fe5b3308f5eaa</t>
+  </si>
+  <si>
+    <t>The C3S dataset is a newer version of the CCI dataset.</t>
+  </si>
+  <si>
+    <t>variable=mole_concentration_of_ozone_in_air,
+processing_level=level_3,
+vertical_aggregation=vertical_profiles_from_limb_sensors,
+sensor=ace,
+version=v0002</t>
+  </si>
+  <si>
+    <t>variable=mole_concentration_of_ozone_in_air,
+processing_level=level_3,
+vertical_aggregation=vertical_profiles_from_limb_sensors,
+sensor=gomos,
+version=v0001</t>
+  </si>
+  <si>
+    <t>variable=mole_concentration_of_ozone_in_air,
+processing_level=level_3,
+vertical_aggregation=vertical_profiles_from_limb_sensors,
+sensor=mipas,
+version=v0002</t>
+  </si>
+  <si>
+    <t>variable=mole_concentration_of_ozone_in_air,
+processing_level=level_3,
+vertical_aggregation=vertical_profiles_from_limb_sensors,
+sensor=osiris,
+version=v0002</t>
+  </si>
+  <si>
+    <t>variable=mole_concentration_of_ozone_in_air,
+processing_level=level_3,
+vertical_aggregation=vertical_profiles_from_limb_sensors,
+sensor=sciamachy,
+version=v0001</t>
+  </si>
+  <si>
+    <t>variable=mole_concentration_of_ozone_in_air,
+processing_level=level_3,
+vertical_aggregation=vertical_profiles_from_limb_sensors,
+sensor=smr,
+version=v0001</t>
+  </si>
+  <si>
+    <t>processing_level=level_3,
+variable=mole_content_of_ozone_in_atmospheric_layer,
+vertical_aggregation=vertical_profiles_from_nadir_sensors,
+sensor=merged_np,
+version=v0100</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/cb54bd70826842a9acf658ebabe4a104</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/ccbeb356a88847058159049678fe5c35</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/b431fbecf73c4442ad5d7bcf80929b03</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/4eb4e801424a47f7b77434291921f889</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/fe651dbef5d44248bef70906f4b3d12b</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/add104f4c4454b629dbc7648efaa1b50</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/f428fffb26cf4cd5b97dfb6381cb16bb</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/4e106bb70a6b42d8a5a86c4635c855b9</t>
+  </si>
+  <si>
+    <t>variable=mole_concentration_of_ozone_in_air,
+processing_level=level_3,
+vertical_aggregation=vertical_profiles_from_limb_sensors,
+sensor=smr,
+version=v0002</t>
+  </si>
+  <si>
+    <t>Vegetation Parameters</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.24381/cds.7e59b01a</t>
+  </si>
+  <si>
+    <t>31/06/2020</t>
+  </si>
+  <si>
+    <t>https://catalogue.ceda.ac.uk/uuid/34e4bfe402c048c783e64eac0f0bca37</t>
+  </si>
+  <si>
+    <t>The C3S and CCI datasets are defined and generated by approximately the same teams, but use different algorithms. Validation in CCI has shown that the algorithm used in CCI (OptiSail) outperforms the algorithm used by C3S (TIP) in many ways.</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1888,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1334,6 +1933,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1371,9 +1971,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1411,7 +2011,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1517,7 +2117,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1659,7 +2259,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1667,42 +2267,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC0B67C-1229-4907-A814-DF79422D0B81}">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
+      <selection activeCell="I145" sqref="I145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" style="6" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="42.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.140625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7265625" customWidth="1"/>
+    <col min="5" max="5" width="23.453125" customWidth="1"/>
+    <col min="6" max="6" width="23.7265625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="30.453125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="30.453125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="42.81640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" customWidth="1"/>
+    <col min="12" max="12" width="23.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.1796875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="14" t="s">
@@ -1712,7 +2312,7 @@
       <c r="K1" s="3"/>
       <c r="M1" s="17"/>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1731,8 +2331,8 @@
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="27"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="15" t="s">
         <v>10</v>
       </c>
@@ -1749,7 +2349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1790,7 +2390,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1798,7 +2398,7 @@
         <v>42370</v>
       </c>
       <c r="C4" s="18">
-        <v>44196</v>
+        <v>44926</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -1831,11 +2431,11 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
     </row>
-    <row r="6" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1876,7 +2476,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>33</v>
       </c>
@@ -1917,7 +2517,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
@@ -1958,11 +2558,11 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2003,7 +2603,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2044,7 +2644,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2085,7 +2685,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2126,7 +2726,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2167,7 +2767,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2208,7 +2808,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2249,7 +2849,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2290,7 +2890,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2331,7 +2931,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2372,7 +2972,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2413,7 +3013,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -2454,7 +3054,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2495,7 +3095,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -2536,7 +3136,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -2577,7 +3177,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -2618,7 +3218,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -2659,7 +3259,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2700,7 +3300,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -2741,7 +3341,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2782,7 +3382,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -2823,7 +3423,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2864,7 +3464,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2905,11 +3505,11 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
     </row>
-    <row r="34" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -2950,7 +3550,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -2991,11 +3591,11 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
     </row>
-    <row r="37" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -3036,7 +3636,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -3077,7 +3677,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -3118,7 +3718,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -3159,7 +3759,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -3200,7 +3800,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -3241,7 +3841,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -3282,7 +3882,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -3323,7 +3923,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -3364,7 +3964,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -3405,7 +4005,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -3446,7 +4046,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -3487,7 +4087,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -3528,7 +4128,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -3569,7 +4169,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -3610,7 +4210,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -3651,7 +4251,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -3692,12 +4292,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="10"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
     </row>
-    <row r="55" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>101</v>
       </c>
@@ -3738,7 +4338,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -3779,7 +4379,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>101</v>
       </c>
@@ -3820,7 +4420,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>101</v>
       </c>
@@ -3861,7 +4461,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -3902,7 +4502,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>101</v>
       </c>
@@ -3943,7 +4543,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -3984,7 +4584,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>101</v>
       </c>
@@ -4025,7 +4625,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>101</v>
       </c>
@@ -4066,7 +4666,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -4107,7 +4707,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -4148,7 +4748,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -4189,7 +4789,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>101</v>
       </c>
@@ -4230,7 +4830,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>101</v>
       </c>
@@ -4271,7 +4871,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -4312,7 +4912,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>101</v>
       </c>
@@ -4353,7 +4953,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>101</v>
       </c>
@@ -4394,19 +4994,19 @@
         <v>251</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
     </row>
-    <row r="73" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>137</v>
       </c>
       <c r="B73" s="19">
         <v>35677</v>
       </c>
-      <c r="C73" s="19">
-        <v>45016</v>
+      <c r="C73" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>178</v>
@@ -4439,15 +5039,15 @@
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>137</v>
       </c>
       <c r="B74" s="19">
         <v>35677</v>
       </c>
-      <c r="C74" s="19">
-        <v>45016</v>
+      <c r="C74" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>179</v>
@@ -4480,15 +5080,15 @@
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>137</v>
       </c>
       <c r="B75" s="19">
         <v>35677</v>
       </c>
-      <c r="C75" s="19">
-        <v>45016</v>
+      <c r="C75" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>180</v>
@@ -4521,15 +5121,15 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>137</v>
       </c>
       <c r="B76" s="19">
         <v>35677</v>
       </c>
-      <c r="C76" s="19">
-        <v>45016</v>
+      <c r="C76" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>181</v>
@@ -4562,15 +5162,15 @@
         <v>258</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>137</v>
       </c>
       <c r="B77" s="19">
         <v>35677</v>
       </c>
-      <c r="C77" s="19">
-        <v>45016</v>
+      <c r="C77" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>182</v>
@@ -4603,15 +5203,15 @@
         <v>258</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>137</v>
       </c>
       <c r="B78" s="19">
         <v>35677</v>
       </c>
-      <c r="C78" s="19">
-        <v>45016</v>
+      <c r="C78" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>183</v>
@@ -4644,14 +5244,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
-      <c r="H79" s="11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="H79" s="11"/>
+    </row>
+    <row r="80" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>140</v>
       </c>
@@ -4659,7 +5257,7 @@
         <v>37347</v>
       </c>
       <c r="C80" s="19">
-        <v>44255</v>
+        <v>44926</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>14</v>
@@ -4677,10 +5275,10 @@
         <v>143</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>287</v>
+        <v>315</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>144</v>
+        <v>14</v>
       </c>
       <c r="K80" t="s">
         <v>19</v>
@@ -4692,7 +5290,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>140</v>
       </c>
@@ -4700,7 +5298,7 @@
         <v>37347</v>
       </c>
       <c r="C81" s="19">
-        <v>44255</v>
+        <v>44926</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>14</v>
@@ -4712,16 +5310,16 @@
         <v>141</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>142</v>
+        <v>317</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>143</v>
+        <v>318</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>145</v>
+        <v>14</v>
       </c>
       <c r="K81" t="s">
         <v>19</v>
@@ -4730,21 +5328,21 @@
         <v>141</v>
       </c>
       <c r="M81" s="8" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A82" s="10" t="s">
-        <v>300</v>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>140</v>
       </c>
       <c r="B82" s="19">
-        <v>33604</v>
+        <v>37347</v>
       </c>
       <c r="C82" s="19">
-        <v>44652</v>
+        <v>44926</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>301</v>
+        <v>14</v>
       </c>
       <c r="E82" t="s">
         <v>15</v>
@@ -4752,17 +5350,17 @@
       <c r="F82" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G82" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H82" s="12" t="s">
-        <v>82</v>
+      <c r="G82" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="H82" s="11" t="s">
+        <v>143</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>302</v>
+        <v>144</v>
       </c>
       <c r="K82" t="s">
         <v>19</v>
@@ -4771,18 +5369,18 @@
         <v>141</v>
       </c>
       <c r="M82" s="8" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B83" s="19">
-        <v>43009</v>
+        <v>37347</v>
       </c>
       <c r="C83" s="19">
-        <v>44469</v>
+        <v>44926</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>14</v>
@@ -4794,16 +5392,16 @@
         <v>141</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K83" t="s">
         <v>19</v>
@@ -4812,107 +5410,107 @@
         <v>141</v>
       </c>
       <c r="M83" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B84" s="19">
+        <v>33604</v>
+      </c>
+      <c r="C84" s="19">
+        <v>44652</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E84" t="s">
+        <v>15</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H84" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J84" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="K84" t="s">
+        <v>19</v>
+      </c>
+      <c r="L84" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="M84" s="8" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" s="19">
+        <v>43009</v>
+      </c>
+      <c r="C85" s="19">
+        <v>44469</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E85" t="s">
+        <v>15</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G85" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="H85" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="K85" t="s">
+        <v>19</v>
+      </c>
+      <c r="L85" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="M85" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
-    </row>
-    <row r="85" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>137</v>
-      </c>
-      <c r="B85" s="19">
-        <v>35677</v>
-      </c>
-      <c r="C85" s="19">
-        <v>45016</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E85" t="s">
-        <v>15</v>
-      </c>
-      <c r="F85" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G85" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="H85" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="I85" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K85" t="s">
-        <v>19</v>
-      </c>
-      <c r="L85" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M85" s="8" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>137</v>
-      </c>
-      <c r="B86" s="19">
-        <v>35677</v>
-      </c>
-      <c r="C86" s="19">
-        <v>45016</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E86" t="s">
-        <v>15</v>
-      </c>
-      <c r="F86" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G86" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H86" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I86" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K86" t="s">
-        <v>19</v>
-      </c>
-      <c r="L86" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="M86" s="8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B86" s="19"/>
+      <c r="C86" s="19"/>
+    </row>
+    <row r="87" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>137</v>
       </c>
       <c r="B87" s="19">
         <v>35677</v>
       </c>
-      <c r="C87" s="19">
-        <v>45016</v>
+      <c r="C87" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E87" t="s">
         <v>15</v>
@@ -4920,14 +5518,14 @@
       <c r="F87" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G87" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H87" s="12" t="s">
-        <v>44</v>
+      <c r="G87" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="H87" s="11" t="s">
+        <v>299</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>14</v>
@@ -4939,21 +5537,21 @@
         <v>138</v>
       </c>
       <c r="M87" s="8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>137</v>
       </c>
       <c r="B88" s="19">
         <v>35677</v>
       </c>
-      <c r="C88" s="19">
-        <v>45016</v>
+      <c r="C88" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E88" t="s">
         <v>15</v>
@@ -4961,14 +5559,14 @@
       <c r="F88" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G88" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H88" s="12" t="s">
-        <v>44</v>
+      <c r="G88" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="H88" s="11" t="s">
+        <v>336</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>14</v>
@@ -4980,21 +5578,21 @@
         <v>138</v>
       </c>
       <c r="M88" s="8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>137</v>
       </c>
       <c r="B89" s="19">
         <v>35677</v>
       </c>
-      <c r="C89" s="19">
-        <v>45016</v>
+      <c r="C89" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E89" t="s">
         <v>15</v>
@@ -5002,14 +5600,14 @@
       <c r="F89" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G89" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H89" s="12" t="s">
-        <v>44</v>
+      <c r="G89" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="H89" s="11" t="s">
+        <v>336</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>14</v>
@@ -5021,21 +5619,21 @@
         <v>138</v>
       </c>
       <c r="M89" s="8" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>137</v>
       </c>
       <c r="B90" s="19">
         <v>35677</v>
       </c>
-      <c r="C90" s="19">
-        <v>45016</v>
+      <c r="C90" s="19" t="s">
+        <v>334</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E90" t="s">
         <v>15</v>
@@ -5043,14 +5641,14 @@
       <c r="F90" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G90" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H90" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="I90" s="16" t="s">
-        <v>237</v>
+      <c r="G90" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="H90" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>239</v>
       </c>
       <c r="J90" s="4" t="s">
         <v>14</v>
@@ -5062,11 +5660,1949 @@
         <v>138</v>
       </c>
       <c r="M90" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>137</v>
+      </c>
+      <c r="B91" s="19">
+        <v>35677</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E91" t="s">
+        <v>15</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K91" t="s">
+        <v>19</v>
+      </c>
+      <c r="L91" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="M91" s="8" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" s="19">
+        <v>35677</v>
+      </c>
+      <c r="C92" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E92" t="s">
+        <v>15</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G92" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="H92" s="11" t="s">
+        <v>336</v>
+      </c>
+      <c r="I92" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K92" t="s">
+        <v>19</v>
+      </c>
+      <c r="L92" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="M92" s="8" t="s">
         <v>292</v>
       </c>
     </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G93" s="8"/>
+    </row>
+    <row r="94" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>303</v>
+      </c>
+      <c r="B94" s="22">
+        <v>36526</v>
+      </c>
+      <c r="C94" s="22">
+        <v>36891</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E94" t="s">
+        <v>15</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="G94" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H94" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="I94" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K94" t="s">
+        <v>19</v>
+      </c>
+      <c r="L94" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="M94" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>308</v>
+      </c>
+      <c r="B96" s="22">
+        <v>34335</v>
+      </c>
+      <c r="C96" s="22">
+        <v>45077</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E96" t="s">
+        <v>15</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="G96" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="H96" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="I96" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K96" t="s">
+        <v>19</v>
+      </c>
+      <c r="L96" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="M96" s="8" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>320</v>
+      </c>
+      <c r="B98" s="22">
+        <v>34851</v>
+      </c>
+      <c r="C98" s="22">
+        <v>44196</v>
+      </c>
+      <c r="D98" t="s">
+        <v>322</v>
+      </c>
+      <c r="E98" t="s">
+        <v>15</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="H98" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K98" t="s">
+        <v>19</v>
+      </c>
+      <c r="L98" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="M98" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>320</v>
+      </c>
+      <c r="B99" s="22">
+        <v>44197</v>
+      </c>
+      <c r="C99" s="22">
+        <v>45291</v>
+      </c>
+      <c r="D99" t="s">
+        <v>327</v>
+      </c>
+      <c r="E99" t="s">
+        <v>15</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G99" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="H99" s="11" t="s">
+        <v>332</v>
+      </c>
+      <c r="I99" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="J99" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K99" t="s">
+        <v>19</v>
+      </c>
+      <c r="L99" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="M99" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="174" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>321</v>
+      </c>
+      <c r="B100" s="22">
+        <v>33873</v>
+      </c>
+      <c r="C100" s="22">
+        <v>45005</v>
+      </c>
+      <c r="D100" t="s">
+        <v>422</v>
+      </c>
+      <c r="E100" t="s">
+        <v>15</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="G100" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H100" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I100" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="J100" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K100" t="s">
+        <v>19</v>
+      </c>
+      <c r="L100" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="M100" s="8" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>337</v>
+      </c>
+      <c r="B102" s="22">
+        <v>37530</v>
+      </c>
+      <c r="C102" s="22">
+        <v>40482</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="E102" t="s">
+        <v>15</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G102" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H102" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I102" s="16" t="s">
+        <v>341</v>
+      </c>
+      <c r="J102" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K102" t="s">
+        <v>19</v>
+      </c>
+      <c r="L102" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M102" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>337</v>
+      </c>
+      <c r="B103" s="22">
+        <v>40483</v>
+      </c>
+      <c r="C103" s="22">
+        <v>43951</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="E103" t="s">
+        <v>15</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G103" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H103" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="J103" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K103" t="s">
+        <v>19</v>
+      </c>
+      <c r="L103" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M103" s="8" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>337</v>
+      </c>
+      <c r="B104" s="22">
+        <v>44105</v>
+      </c>
+      <c r="C104" s="22">
+        <v>45322</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="E104" t="s">
+        <v>15</v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="H104" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="I104" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="J104" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K104" t="s">
+        <v>19</v>
+      </c>
+      <c r="L104" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M104" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>343</v>
+      </c>
+      <c r="B105" s="22">
+        <v>37408</v>
+      </c>
+      <c r="C105" s="22">
+        <v>44196</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E105" t="s">
+        <v>15</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G105" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H105" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="J105" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K105" t="s">
+        <v>19</v>
+      </c>
+      <c r="L105" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M105" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A106" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B106" s="22">
+        <v>37408</v>
+      </c>
+      <c r="C106" s="22">
+        <v>44196</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E106" t="s">
+        <v>353</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G106" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H106" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I106" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="J106" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K106" t="s">
+        <v>19</v>
+      </c>
+      <c r="L106" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M106" s="8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="B107" s="22">
+        <v>37409</v>
+      </c>
+      <c r="C107" s="22">
+        <v>44197</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E107" t="s">
+        <v>15</v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G107" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H107" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I107" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="J107" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K107" t="s">
+        <v>353</v>
+      </c>
+      <c r="L107" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M107" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="B108" s="22">
+        <v>28788</v>
+      </c>
+      <c r="C108" s="22">
+        <v>44196</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="E108" t="s">
+        <v>15</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H108" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I108" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="J108" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K108" t="s">
+        <v>19</v>
+      </c>
+      <c r="L108" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M108" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>356</v>
+      </c>
+      <c r="B109" s="22">
+        <v>28789</v>
+      </c>
+      <c r="C109" s="22">
+        <v>44197</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E109" t="s">
+        <v>353</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G109" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H109" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I109" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="J109" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K109" t="s">
+        <v>19</v>
+      </c>
+      <c r="L109" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M109" s="8" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>351</v>
+      </c>
+      <c r="B110" s="22">
+        <v>28788</v>
+      </c>
+      <c r="C110" s="22">
+        <v>44196</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="E110" t="s">
+        <v>15</v>
+      </c>
+      <c r="F110" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="G110" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H110" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I110" t="s">
+        <v>356</v>
+      </c>
+      <c r="J110" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K110" t="s">
+        <v>353</v>
+      </c>
+      <c r="L110" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="M110" s="8" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>372</v>
+      </c>
+      <c r="B112" s="22">
+        <v>37438</v>
+      </c>
+      <c r="C112" s="22">
+        <v>43100</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E112" t="s">
+        <v>365</v>
+      </c>
+      <c r="F112" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="G112" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H112" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I112" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="J112" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K112" t="s">
+        <v>19</v>
+      </c>
+      <c r="L112" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="M112" s="8" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>369</v>
+      </c>
+      <c r="B113" s="22">
+        <v>37439</v>
+      </c>
+      <c r="C113" s="22">
+        <v>43100</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="E113" t="s">
+        <v>370</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="G113" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="H113" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="I113" t="s">
+        <v>372</v>
+      </c>
+      <c r="J113" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K113" t="s">
+        <v>365</v>
+      </c>
+      <c r="L113" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="M113" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A114" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B114" s="22">
+        <v>37439</v>
+      </c>
+      <c r="C114" s="22">
+        <v>43100</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="E114" t="s">
+        <v>370</v>
+      </c>
+      <c r="F114" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="G114" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="H114" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="I114" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="J114" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K114" t="s">
+        <v>19</v>
+      </c>
+      <c r="L114" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="M114" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>379</v>
+      </c>
+      <c r="B116" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C116" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="E116" t="s">
+        <v>370</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G116" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="H116" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="I116" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="J116" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K116" t="s">
+        <v>19</v>
+      </c>
+      <c r="L116" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M116" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>379</v>
+      </c>
+      <c r="B117" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C117" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="E117" t="s">
+        <v>370</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G117" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="H117" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="I117" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="J117" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K117" t="s">
+        <v>19</v>
+      </c>
+      <c r="L117" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M117" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>379</v>
+      </c>
+      <c r="B118" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C118" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="E118" t="s">
+        <v>370</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G118" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="H118" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="I118" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="J118" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K118" t="s">
+        <v>19</v>
+      </c>
+      <c r="L118" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M118" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>379</v>
+      </c>
+      <c r="B119" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C119" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="E119" t="s">
+        <v>370</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G119" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H119" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="I119" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="J119" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K119" t="s">
+        <v>19</v>
+      </c>
+      <c r="L119" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M119" s="8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>379</v>
+      </c>
+      <c r="B120" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C120" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="E120" t="s">
+        <v>370</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G120" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="H120" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="I120" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="J120" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K120" t="s">
+        <v>19</v>
+      </c>
+      <c r="L120" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M120" s="8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>379</v>
+      </c>
+      <c r="B121" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C121" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E121" t="s">
+        <v>370</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G121" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H121" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="I121" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="J121" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K121" t="s">
+        <v>19</v>
+      </c>
+      <c r="L121" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M121" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>379</v>
+      </c>
+      <c r="B122" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C122" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="E122" t="s">
+        <v>370</v>
+      </c>
+      <c r="F122" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G122" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="H122" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="I122" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="J122" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K122" t="s">
+        <v>19</v>
+      </c>
+      <c r="L122" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M122" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>379</v>
+      </c>
+      <c r="B123" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C123" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="E123" t="s">
+        <v>370</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G123" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="H123" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="I123" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="J123" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K123" t="s">
+        <v>19</v>
+      </c>
+      <c r="L123" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M123" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>379</v>
+      </c>
+      <c r="B124" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C124" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="E124" t="s">
+        <v>370</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G124" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="H124" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="I124" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="J124" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K124" t="s">
+        <v>19</v>
+      </c>
+      <c r="L124" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M124" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>379</v>
+      </c>
+      <c r="B125" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C125" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="E125" t="s">
+        <v>370</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G125" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H125" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="I125" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="J125" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K125" t="s">
+        <v>19</v>
+      </c>
+      <c r="L125" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M125" s="8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>379</v>
+      </c>
+      <c r="B126" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C126" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="E126" t="s">
+        <v>370</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G126" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="H126" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="I126" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="J126" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K126" t="s">
+        <v>19</v>
+      </c>
+      <c r="L126" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M126" s="8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>379</v>
+      </c>
+      <c r="B127" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C127" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D127" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E127" t="s">
+        <v>370</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G127" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H127" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="I127" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="J127" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K127" t="s">
+        <v>19</v>
+      </c>
+      <c r="L127" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M127" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>379</v>
+      </c>
+      <c r="B128" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C128" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="E128" t="s">
+        <v>370</v>
+      </c>
+      <c r="F128" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G128" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="H128" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="I128" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="J128" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K128" t="s">
+        <v>19</v>
+      </c>
+      <c r="L128" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M128" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>379</v>
+      </c>
+      <c r="B129" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C129" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="E129" t="s">
+        <v>370</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G129" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="H129" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="I129" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="J129" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K129" t="s">
+        <v>19</v>
+      </c>
+      <c r="L129" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M129" s="8" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>379</v>
+      </c>
+      <c r="B130" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C130" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="E130" t="s">
+        <v>370</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G130" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="H130" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="I130" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="J130" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K130" t="s">
+        <v>19</v>
+      </c>
+      <c r="L130" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M130" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>379</v>
+      </c>
+      <c r="B131" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C131" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E131" t="s">
+        <v>370</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G131" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H131" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="I131" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="J131" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K131" t="s">
+        <v>19</v>
+      </c>
+      <c r="L131" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M131" s="8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>379</v>
+      </c>
+      <c r="B132" s="22">
+        <v>33455</v>
+      </c>
+      <c r="C132" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="E132" t="s">
+        <v>370</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G132" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="H132" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="I132" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="J132" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K132" t="s">
+        <v>19</v>
+      </c>
+      <c r="L132" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M132" s="8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>379</v>
+      </c>
+      <c r="B133" s="22">
+        <v>44927</v>
+      </c>
+      <c r="C133" s="22">
+        <v>45422</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="E133" t="s">
+        <v>370</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="G133" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="H133" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="I133" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="J133" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K133" t="s">
+        <v>19</v>
+      </c>
+      <c r="L133" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M133" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>424</v>
+      </c>
+      <c r="B135" s="22">
+        <v>34881</v>
+      </c>
+      <c r="C135" s="22">
+        <v>45046</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="E135" t="s">
+        <v>370</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G135" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H135" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I135" s="16" t="s">
+        <v>427</v>
+      </c>
+      <c r="J135" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K135" t="s">
+        <v>19</v>
+      </c>
+      <c r="L135" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M135" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>424</v>
+      </c>
+      <c r="B136" s="22">
+        <v>38018</v>
+      </c>
+      <c r="C136" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="E136" t="s">
+        <v>370</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G136" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H136" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I136" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="J136" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K136" t="s">
+        <v>19</v>
+      </c>
+      <c r="L136" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M136" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>424</v>
+      </c>
+      <c r="B137" s="22">
+        <v>37469</v>
+      </c>
+      <c r="C137" s="22">
+        <v>40908</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="E137" t="s">
+        <v>370</v>
+      </c>
+      <c r="F137" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G137" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H137" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I137" s="16" t="s">
+        <v>438</v>
+      </c>
+      <c r="J137" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K137" t="s">
+        <v>19</v>
+      </c>
+      <c r="L137" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M137" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>424</v>
+      </c>
+      <c r="B138" s="22">
+        <v>37438</v>
+      </c>
+      <c r="C138" s="22">
+        <v>40908</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="E138" t="s">
+        <v>370</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G138" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H138" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I138" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="J138" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K138" t="s">
+        <v>19</v>
+      </c>
+      <c r="L138" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M138" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>424</v>
+      </c>
+      <c r="B139" s="22">
+        <v>37196</v>
+      </c>
+      <c r="C139" s="22">
+        <v>44926</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="E139" t="s">
+        <v>370</v>
+      </c>
+      <c r="F139" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G139" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H139" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I139" s="16" t="s">
+        <v>442</v>
+      </c>
+      <c r="J139" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K139" t="s">
+        <v>19</v>
+      </c>
+      <c r="L139" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M139" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>424</v>
+      </c>
+      <c r="B140" s="22">
+        <v>37469</v>
+      </c>
+      <c r="C140" s="22">
+        <v>40908</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="E140" t="s">
+        <v>370</v>
+      </c>
+      <c r="F140" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G140" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H140" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I140" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="J140" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K140" t="s">
+        <v>19</v>
+      </c>
+      <c r="L140" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M140" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>424</v>
+      </c>
+      <c r="B141" s="22">
+        <v>37073</v>
+      </c>
+      <c r="C141" s="22">
+        <v>41882</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E141" t="s">
+        <v>370</v>
+      </c>
+      <c r="F141" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G141" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H141" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I141" s="16" t="s">
+        <v>440</v>
+      </c>
+      <c r="J141" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K141" t="s">
+        <v>19</v>
+      </c>
+      <c r="L141" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M141" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>424</v>
+      </c>
+      <c r="B142" s="22"/>
+      <c r="C142" s="22"/>
+      <c r="D142" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="E142" t="s">
+        <v>370</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G142" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H142" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I142" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="J142" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K142" t="s">
+        <v>19</v>
+      </c>
+      <c r="L142" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M142" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>424</v>
+      </c>
+      <c r="B143" s="22">
+        <v>34881</v>
+      </c>
+      <c r="C143" s="22">
+        <v>44500</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E143" t="s">
+        <v>370</v>
+      </c>
+      <c r="F143" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="G143" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H143" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="I143" s="16" t="s">
+        <v>439</v>
+      </c>
+      <c r="J143" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K143" t="s">
+        <v>19</v>
+      </c>
+      <c r="L143" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="M143" s="8" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D144" s="4"/>
+    </row>
+    <row r="145" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>446</v>
+      </c>
+      <c r="B145" s="22">
+        <v>29830</v>
+      </c>
+      <c r="C145" t="s">
+        <v>447</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E145" t="s">
+        <v>370</v>
+      </c>
+      <c r="F145" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="G145" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="H145" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I145" s="16" t="s">
+        <v>448</v>
+      </c>
+      <c r="J145" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K145" t="s">
+        <v>19</v>
+      </c>
+      <c r="L145" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="M145" s="8" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D146" s="4"/>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D147" s="4"/>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D148" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="L1:L90" xr:uid="{9CC0B67C-1229-4907-A814-DF79422D0B81}"/>
+  <autoFilter ref="L1:L92" xr:uid="{9CC0B67C-1229-4907-A814-DF79422D0B81}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:G2"/>
@@ -5084,10 +7620,21 @@
     <hyperlink ref="I39" r:id="rId8" display="http://catalogue.ceda.ac.uk/uuid/9255faeb392f41debf5402caa40dada8" xr:uid="{33D8A6EC-1721-4D70-A807-90A9DC0F92B0}"/>
     <hyperlink ref="I40" r:id="rId9" display="http://catalogue.ceda.ac.uk/uuid/e61704b00267405082fbd41bb710dd74" xr:uid="{06FBE9A3-0C52-45E7-A072-ADF695817CB1}"/>
     <hyperlink ref="I57" r:id="rId10" xr:uid="{22CAB548-7850-41A6-A99E-34D32F625495}"/>
-    <hyperlink ref="A82" r:id="rId11" display="https://doi.org/10.24381/cds.056d0df7" xr:uid="{77B16774-B5C1-4B68-B8D8-66D71A016F6E}"/>
+    <hyperlink ref="A84" r:id="rId11" display="https://doi.org/10.24381/cds.056d0df7" xr:uid="{77B16774-B5C1-4B68-B8D8-66D71A016F6E}"/>
+    <hyperlink ref="I102" r:id="rId12" xr:uid="{FEB01A84-4724-4528-BBE6-6A672EF16375}"/>
+    <hyperlink ref="A114" r:id="rId13" xr:uid="{C040648D-618B-4F46-AE41-B50586C6D7F7}"/>
+    <hyperlink ref="A108" r:id="rId14" xr:uid="{64775FEC-C3F8-48EB-88F4-7DBA09DE89F9}"/>
+    <hyperlink ref="A107" r:id="rId15" xr:uid="{8BD21AAD-9633-4232-A3E2-86BDE2443D61}"/>
+    <hyperlink ref="I135" r:id="rId16" xr:uid="{BDDFA5AF-1977-44C5-BCB0-91FD1402009E}"/>
+    <hyperlink ref="I137" r:id="rId17" xr:uid="{BDEDEFCF-A555-472E-9706-1AE567A01700}"/>
+    <hyperlink ref="I143" r:id="rId18" xr:uid="{22A88BF9-38BF-4AD8-B7DD-41EB2ECEB1F1}"/>
+    <hyperlink ref="I141" r:id="rId19" xr:uid="{93ED3F05-B542-43CF-B31F-B333FB17814F}"/>
+    <hyperlink ref="I139" r:id="rId20" xr:uid="{13FC54EB-DE3C-4179-AFA4-C1747B414A0A}"/>
+    <hyperlink ref="I138" r:id="rId21" xr:uid="{87679DBA-7FAA-4B74-AAD7-6E4D869079F3}"/>
+    <hyperlink ref="I145" r:id="rId22" xr:uid="{45452A3D-3C2A-44E8-9ECB-DDB7F746AC92}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -5095,22 +7642,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B35E6D-763F-4C40-91D2-473BE7766F62}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="105.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="105.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
@@ -5118,7 +7665,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -5126,7 +7673,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -5134,7 +7681,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -5142,7 +7689,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -5150,7 +7697,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -5158,7 +7705,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -5166,7 +7713,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -5174,7 +7721,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>163</v>
       </c>
@@ -5182,7 +7729,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -5190,7 +7737,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -5198,7 +7745,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -5206,7 +7753,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -5214,7 +7761,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -5222,7 +7769,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>170</v>
       </c>
@@ -5230,7 +7777,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -5238,7 +7785,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>174</v>
       </c>
@@ -5246,7 +7793,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>176</v>
       </c>

</xml_diff>

<commit_message>
Remove blank lines before relationships for https://doi.org/10.24381/cds.8e0e4724
</commit_message>
<xml_diff>
--- a/EEE2000-metadata_mapping.xlsx
+++ b/EEE2000-metadata_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amw23\Documents\GitHub\cci_data_bridge_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajw22/git/cci_data_bridge_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30529C78-4B94-42A9-BF27-277C550CC532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804A3DE7-350E-8D49-9FFC-08F9198AAE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B9DA58AC-C110-4CBA-A19B-6F37B44EEA38}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26040" windowHeight="17500" xr2:uid="{B9DA58AC-C110-4CBA-A19B-6F37B44EEA38}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="445">
   <si>
     <t>Dataset 1</t>
   </si>
@@ -1358,10 +1358,6 @@
   </si>
   <si>
     <t>C3S</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-IsIdenticalTo</t>
   </si>
   <si>
     <t>https://doi.org/10.5676/EUM_SAF_CM/COMBI/V001</t>
@@ -2259,28 +2255,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC0B67C-1229-4907-A814-DF79422D0B81}">
   <dimension ref="A1:M148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="48" zoomScaleNormal="48" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="B110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.54296875" customWidth="1"/>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="38.7265625" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" customWidth="1"/>
-    <col min="6" max="6" width="23.7265625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="30.453125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="30.453125" style="12" customWidth="1"/>
-    <col min="9" max="9" width="42.81640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="19.26953125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.26953125" customWidth="1"/>
-    <col min="12" max="12" width="23.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="47.1796875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="30.1640625" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="30.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="30.5" style="12" customWidth="1"/>
+    <col min="9" max="9" width="42.83203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="47.1640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2298,7 @@
       <c r="K1" s="3"/>
       <c r="M1" s="17"/>
     </row>
-    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -2339,7 +2335,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2380,7 +2376,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2421,11 +2417,11 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
     </row>
-    <row r="6" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -2466,7 +2462,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>33</v>
       </c>
@@ -2507,7 +2503,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
@@ -2548,11 +2544,11 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
     </row>
-    <row r="10" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -2593,7 +2589,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2634,7 +2630,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2675,7 +2671,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -2716,7 +2712,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2757,7 +2753,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -2798,7 +2794,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -2839,7 +2835,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2880,7 +2876,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2921,7 +2917,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -2962,7 +2958,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -3003,7 +2999,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -3044,7 +3040,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -3085,7 +3081,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -3126,7 +3122,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -3167,7 +3163,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>43</v>
       </c>
@@ -3208,7 +3204,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -3249,7 +3245,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -3290,7 +3286,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3331,7 +3327,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -3372,7 +3368,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -3413,7 +3409,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -3454,7 +3450,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -3495,11 +3491,11 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
     </row>
-    <row r="34" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -3540,7 +3536,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -3581,11 +3577,11 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
     </row>
-    <row r="37" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -3626,7 +3622,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>75</v>
       </c>
@@ -3667,7 +3663,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>75</v>
       </c>
@@ -3708,7 +3704,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -3749,7 +3745,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>75</v>
       </c>
@@ -3790,7 +3786,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -3831,7 +3827,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -3872,7 +3868,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -3913,7 +3909,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -3954,7 +3950,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -3995,7 +3991,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -4036,7 +4032,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -4077,7 +4073,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -4118,7 +4114,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -4159,7 +4155,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -4200,7 +4196,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -4241,7 +4237,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -4282,12 +4278,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="10"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
     </row>
-    <row r="55" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>101</v>
       </c>
@@ -4328,7 +4324,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -4369,7 +4365,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>101</v>
       </c>
@@ -4410,7 +4406,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>101</v>
       </c>
@@ -4451,7 +4447,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -4492,7 +4488,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>101</v>
       </c>
@@ -4533,7 +4529,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>101</v>
       </c>
@@ -4574,7 +4570,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>101</v>
       </c>
@@ -4615,7 +4611,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>101</v>
       </c>
@@ -4656,7 +4652,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -4697,7 +4693,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -4738,7 +4734,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -4779,7 +4775,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>101</v>
       </c>
@@ -4820,7 +4816,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>101</v>
       </c>
@@ -4861,7 +4857,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -4902,7 +4898,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>101</v>
       </c>
@@ -4943,7 +4939,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>101</v>
       </c>
@@ -4984,11 +4980,11 @@
         <v>251</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
     </row>
-    <row r="73" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>137</v>
       </c>
@@ -5029,7 +5025,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>137</v>
       </c>
@@ -5070,7 +5066,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>137</v>
       </c>
@@ -5111,7 +5107,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>137</v>
       </c>
@@ -5152,7 +5148,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>137</v>
       </c>
@@ -5193,7 +5189,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>137</v>
       </c>
@@ -5234,12 +5230,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
       <c r="H79" s="11"/>
     </row>
-    <row r="80" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>140</v>
       </c>
@@ -5280,7 +5276,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>140</v>
       </c>
@@ -5321,7 +5317,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>140</v>
       </c>
@@ -5362,7 +5358,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>140</v>
       </c>
@@ -5403,7 +5399,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
         <v>300</v>
       </c>
@@ -5444,7 +5440,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="116" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>146</v>
       </c>
@@ -5485,11 +5481,11 @@
         <v>184</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
     </row>
-    <row r="87" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>137</v>
       </c>
@@ -5530,7 +5526,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>137</v>
       </c>
@@ -5571,7 +5567,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>137</v>
       </c>
@@ -5612,7 +5608,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>137</v>
       </c>
@@ -5653,7 +5649,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>137</v>
       </c>
@@ -5694,7 +5690,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>137</v>
       </c>
@@ -5735,10 +5731,10 @@
         <v>292</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>303</v>
       </c>
@@ -5779,11 +5775,11 @@
         <v>307</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B95" s="19"/>
       <c r="C95" s="19"/>
     </row>
-    <row r="96" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>308</v>
       </c>
@@ -5824,7 +5820,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>320</v>
       </c>
@@ -5865,7 +5861,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>320</v>
       </c>
@@ -5906,7 +5902,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="174" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:13" ht="176" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>321</v>
       </c>
@@ -5917,7 +5913,7 @@
         <v>45005</v>
       </c>
       <c r="D100" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E100" t="s">
         <v>15</v>
@@ -5944,14 +5940,14 @@
         <v>323</v>
       </c>
       <c r="M100" s="8" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B101" s="19"/>
       <c r="C101" s="19"/>
     </row>
-    <row r="102" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>336</v>
       </c>
@@ -5992,7 +5988,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>336</v>
       </c>
@@ -6033,7 +6029,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="58" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>336</v>
       </c>
@@ -6074,7 +6070,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>342</v>
       </c>
@@ -6115,7 +6111,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>354</v>
       </c>
@@ -6156,7 +6152,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
         <v>342</v>
       </c>
@@ -6197,7 +6193,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
         <v>342</v>
       </c>
@@ -6238,7 +6234,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>355</v>
       </c>
@@ -6279,7 +6275,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>350</v>
       </c>
@@ -6320,13 +6316,13 @@
         <v>347</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B111" s="19"/>
       <c r="C111" s="19"/>
     </row>
-    <row r="112" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B112" s="19">
         <v>37438</v>
@@ -6365,7 +6361,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>366</v>
       </c>
@@ -6376,7 +6372,7 @@
         <v>43100</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E113" t="s">
         <v>367</v>
@@ -6385,13 +6381,13 @@
         <v>364</v>
       </c>
       <c r="G113" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H113" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I113" t="s">
         <v>368</v>
-      </c>
-      <c r="H113" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="I113" t="s">
-        <v>369</v>
       </c>
       <c r="J113" s="4" t="s">
         <v>14</v>
@@ -6403,10 +6399,10 @@
         <v>364</v>
       </c>
       <c r="M113" s="8" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
         <v>366</v>
       </c>
@@ -6417,7 +6413,7 @@
         <v>43100</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E114" t="s">
         <v>367</v>
@@ -6426,10 +6422,10 @@
         <v>364</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>368</v>
+        <v>41</v>
       </c>
       <c r="H114" s="11" t="s">
-        <v>368</v>
+        <v>41</v>
       </c>
       <c r="I114" s="4" t="s">
         <v>363</v>
@@ -6444,16 +6440,16 @@
         <v>364</v>
       </c>
       <c r="M114" s="8" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
     </row>
-    <row r="116" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B116" s="19">
         <v>33455</v>
@@ -6462,23 +6458,23 @@
         <v>44926</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E116" t="s">
         <v>367</v>
       </c>
       <c r="F116" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="G116" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="H116" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="I116" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="G116" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="H116" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="I116" s="4" t="s">
-        <v>374</v>
-      </c>
       <c r="J116" s="4" t="s">
         <v>14</v>
       </c>
@@ -6486,15 +6482,15 @@
         <v>19</v>
       </c>
       <c r="L116" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M116" s="8" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B117" s="19">
         <v>44927</v>
@@ -6503,23 +6499,23 @@
         <v>45422</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E117" t="s">
         <v>367</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G117" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="H117" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="H117" s="11" t="s">
+      <c r="I117" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="I117" s="4" t="s">
-        <v>382</v>
-      </c>
       <c r="J117" s="4" t="s">
         <v>14</v>
       </c>
@@ -6527,15 +6523,15 @@
         <v>19</v>
       </c>
       <c r="L117" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M117" s="8" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B118" s="19">
         <v>33455</v>
@@ -6544,22 +6540,22 @@
         <v>44926</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E118" t="s">
         <v>367</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G118" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="H118" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="H118" s="11" t="s">
-        <v>390</v>
-      </c>
       <c r="I118" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J118" s="4" t="s">
         <v>14</v>
@@ -6568,15 +6564,15 @@
         <v>19</v>
       </c>
       <c r="L118" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M118" s="8" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B119" s="19">
         <v>44927</v>
@@ -6585,22 +6581,22 @@
         <v>45422</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E119" t="s">
         <v>367</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G119" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="H119" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="H119" s="11" t="s">
-        <v>392</v>
-      </c>
       <c r="I119" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J119" s="4" t="s">
         <v>14</v>
@@ -6609,15 +6605,15 @@
         <v>19</v>
       </c>
       <c r="L119" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M119" s="8" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B120" s="19">
         <v>33455</v>
@@ -6626,22 +6622,22 @@
         <v>44926</v>
       </c>
       <c r="D120" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E120" t="s">
         <v>367</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G120" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="H120" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="H120" s="11" t="s">
-        <v>390</v>
-      </c>
       <c r="I120" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J120" s="4" t="s">
         <v>14</v>
@@ -6650,15 +6646,15 @@
         <v>19</v>
       </c>
       <c r="L120" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M120" s="8" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B121" s="19">
         <v>44927</v>
@@ -6667,22 +6663,22 @@
         <v>45422</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E121" t="s">
         <v>367</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G121" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="H121" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="H121" s="11" t="s">
-        <v>392</v>
-      </c>
       <c r="I121" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J121" s="4" t="s">
         <v>14</v>
@@ -6691,15 +6687,15 @@
         <v>19</v>
       </c>
       <c r="L121" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="122" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B122" s="19">
         <v>33455</v>
@@ -6708,22 +6704,22 @@
         <v>44926</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E122" t="s">
         <v>367</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G122" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="H122" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="H122" s="11" t="s">
-        <v>379</v>
-      </c>
       <c r="I122" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J122" s="4" t="s">
         <v>14</v>
@@ -6732,15 +6728,15 @@
         <v>19</v>
       </c>
       <c r="L122" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M122" s="8" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B123" s="19">
         <v>44927</v>
@@ -6749,22 +6745,22 @@
         <v>45422</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E123" t="s">
         <v>367</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G123" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="H123" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="H123" s="11" t="s">
-        <v>381</v>
-      </c>
       <c r="I123" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J123" s="4" t="s">
         <v>14</v>
@@ -6773,15 +6769,15 @@
         <v>19</v>
       </c>
       <c r="L123" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M123" s="8" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="124" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B124" s="19">
         <v>33455</v>
@@ -6790,22 +6786,22 @@
         <v>44926</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E124" t="s">
         <v>367</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G124" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="H124" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="H124" s="11" t="s">
-        <v>390</v>
-      </c>
       <c r="I124" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J124" s="4" t="s">
         <v>14</v>
@@ -6814,15 +6810,15 @@
         <v>19</v>
       </c>
       <c r="L124" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M124" s="8" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="125" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B125" s="19">
         <v>44927</v>
@@ -6831,22 +6827,22 @@
         <v>45422</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E125" t="s">
         <v>367</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G125" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="H125" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="H125" s="11" t="s">
-        <v>392</v>
-      </c>
       <c r="I125" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J125" s="4" t="s">
         <v>14</v>
@@ -6855,15 +6851,15 @@
         <v>19</v>
       </c>
       <c r="L125" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M125" s="8" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="126" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B126" s="19">
         <v>33455</v>
@@ -6872,22 +6868,22 @@
         <v>44926</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E126" t="s">
         <v>367</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G126" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="H126" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="H126" s="11" t="s">
-        <v>390</v>
-      </c>
       <c r="I126" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J126" s="4" t="s">
         <v>14</v>
@@ -6896,15 +6892,15 @@
         <v>19</v>
       </c>
       <c r="L126" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M126" s="8" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="127" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B127" s="19">
         <v>44927</v>
@@ -6913,22 +6909,22 @@
         <v>45422</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E127" t="s">
         <v>367</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G127" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="H127" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="H127" s="11" t="s">
-        <v>392</v>
-      </c>
       <c r="I127" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J127" s="4" t="s">
         <v>14</v>
@@ -6937,15 +6933,15 @@
         <v>19</v>
       </c>
       <c r="L127" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M127" s="8" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="128" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B128" s="19">
         <v>33455</v>
@@ -6954,22 +6950,22 @@
         <v>44926</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E128" t="s">
         <v>367</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G128" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="H128" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="H128" s="11" t="s">
-        <v>379</v>
-      </c>
       <c r="I128" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="J128" s="4" t="s">
         <v>14</v>
@@ -6978,15 +6974,15 @@
         <v>19</v>
       </c>
       <c r="L128" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M128" s="8" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B129" s="19">
         <v>44927</v>
@@ -6995,22 +6991,22 @@
         <v>45422</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E129" t="s">
         <v>367</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G129" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="H129" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="H129" s="11" t="s">
-        <v>381</v>
-      </c>
       <c r="I129" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="J129" s="4" t="s">
         <v>14</v>
@@ -7019,15 +7015,15 @@
         <v>19</v>
       </c>
       <c r="L129" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M129" s="8" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="130" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B130" s="19">
         <v>33455</v>
@@ -7036,22 +7032,22 @@
         <v>44926</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E130" t="s">
         <v>367</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G130" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="H130" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="H130" s="11" t="s">
-        <v>390</v>
-      </c>
       <c r="I130" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="J130" s="4" t="s">
         <v>14</v>
@@ -7060,15 +7056,15 @@
         <v>19</v>
       </c>
       <c r="L130" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M130" s="8" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="131" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B131" s="19">
         <v>44927</v>
@@ -7077,22 +7073,22 @@
         <v>45422</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E131" t="s">
         <v>367</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G131" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="H131" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="H131" s="11" t="s">
-        <v>392</v>
-      </c>
       <c r="I131" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J131" s="4" t="s">
         <v>14</v>
@@ -7101,15 +7097,15 @@
         <v>19</v>
       </c>
       <c r="L131" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M131" s="8" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="132" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B132" s="19">
         <v>33455</v>
@@ -7118,22 +7114,22 @@
         <v>44926</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E132" t="s">
         <v>367</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G132" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="H132" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="H132" s="11" t="s">
-        <v>390</v>
-      </c>
       <c r="I132" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J132" s="4" t="s">
         <v>14</v>
@@ -7142,15 +7138,15 @@
         <v>19</v>
       </c>
       <c r="L132" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M132" s="8" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="133" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B133" s="19">
         <v>44927</v>
@@ -7159,22 +7155,22 @@
         <v>45422</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E133" t="s">
         <v>367</v>
       </c>
       <c r="F133" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G133" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="H133" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="H133" s="11" t="s">
-        <v>392</v>
-      </c>
       <c r="I133" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="J133" s="4" t="s">
         <v>14</v>
@@ -7183,19 +7179,19 @@
         <v>19</v>
       </c>
       <c r="L133" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M133" s="8" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B134" s="19"/>
       <c r="C134" s="19"/>
     </row>
-    <row r="135" spans="1:13" ht="87" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B135" s="19">
         <v>34881</v>
@@ -7204,39 +7200,39 @@
         <v>45046</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E135" t="s">
         <v>367</v>
       </c>
       <c r="F135" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="G135" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="H135" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="I135" s="16" t="s">
         <v>423</v>
       </c>
-      <c r="G135" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="H135" s="11" t="s">
-        <v>378</v>
-      </c>
-      <c r="I135" s="16" t="s">
+      <c r="J135" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K135" t="s">
+        <v>19</v>
+      </c>
+      <c r="L135" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="M135" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="J135" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K135" t="s">
-        <v>19</v>
-      </c>
-      <c r="L135" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="M135" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="136" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B136" s="19">
         <v>38018</v>
@@ -7245,22 +7241,22 @@
         <v>44926</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E136" t="s">
         <v>367</v>
       </c>
       <c r="F136" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G136" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H136" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I136" s="4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J136" s="4" t="s">
         <v>14</v>
@@ -7269,15 +7265,15 @@
         <v>19</v>
       </c>
       <c r="L136" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M136" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="137" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="137" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B137" s="19">
         <v>37469</v>
@@ -7286,22 +7282,22 @@
         <v>40908</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E137" t="s">
         <v>367</v>
       </c>
       <c r="F137" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G137" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H137" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I137" s="16" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J137" s="4" t="s">
         <v>14</v>
@@ -7310,15 +7306,15 @@
         <v>19</v>
       </c>
       <c r="L137" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M137" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B138" s="19">
         <v>37438</v>
@@ -7327,22 +7323,22 @@
         <v>40908</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E138" t="s">
         <v>367</v>
       </c>
       <c r="F138" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G138" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H138" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I138" s="16" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J138" s="4" t="s">
         <v>14</v>
@@ -7351,15 +7347,15 @@
         <v>19</v>
       </c>
       <c r="L138" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M138" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="139" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B139" s="19">
         <v>37196</v>
@@ -7368,22 +7364,22 @@
         <v>44926</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E139" t="s">
         <v>367</v>
       </c>
       <c r="F139" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G139" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H139" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I139" s="16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J139" s="4" t="s">
         <v>14</v>
@@ -7392,15 +7388,15 @@
         <v>19</v>
       </c>
       <c r="L139" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M139" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="140" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B140" s="19">
         <v>37469</v>
@@ -7409,22 +7405,22 @@
         <v>40908</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E140" t="s">
         <v>367</v>
       </c>
       <c r="F140" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G140" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H140" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I140" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J140" s="4" t="s">
         <v>14</v>
@@ -7433,15 +7429,15 @@
         <v>19</v>
       </c>
       <c r="L140" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M140" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="141" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B141" s="19">
         <v>37073</v>
@@ -7450,22 +7446,22 @@
         <v>41882</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E141" t="s">
         <v>367</v>
       </c>
       <c r="F141" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G141" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H141" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I141" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J141" s="4" t="s">
         <v>14</v>
@@ -7474,15 +7470,15 @@
         <v>19</v>
       </c>
       <c r="L141" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M141" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="142" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" ht="96" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B142" s="19">
         <v>37074</v>
@@ -7491,22 +7487,22 @@
         <v>41882</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E142" t="s">
         <v>367</v>
       </c>
       <c r="F142" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G142" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H142" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I142" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J142" s="4" t="s">
         <v>14</v>
@@ -7515,15 +7511,15 @@
         <v>19</v>
       </c>
       <c r="L142" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M142" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="143" spans="1:13" ht="101.5" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" ht="112" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B143" s="19">
         <v>34881</v>
@@ -7532,22 +7528,22 @@
         <v>44500</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E143" t="s">
         <v>367</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G143" s="8" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H143" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I143" s="16" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J143" s="4" t="s">
         <v>14</v>
@@ -7556,20 +7552,20 @@
         <v>19</v>
       </c>
       <c r="L143" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="M143" s="8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B144" s="19"/>
       <c r="C144" s="19"/>
       <c r="D144" s="4"/>
     </row>
-    <row r="145" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B145" s="19">
         <v>29830</v>
@@ -7584,7 +7580,7 @@
         <v>367</v>
       </c>
       <c r="F145" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G145" s="9" t="s">
         <v>163</v>
@@ -7593,28 +7589,28 @@
         <v>161</v>
       </c>
       <c r="I145" s="16" t="s">
+        <v>443</v>
+      </c>
+      <c r="J145" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K145" t="s">
+        <v>19</v>
+      </c>
+      <c r="L145" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="M145" s="8" t="s">
         <v>444</v>
       </c>
-      <c r="J145" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K145" t="s">
-        <v>19</v>
-      </c>
-      <c r="L145" s="6" t="s">
-        <v>442</v>
-      </c>
-      <c r="M145" s="8" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D146" s="4"/>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D147" s="4"/>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D148" s="4"/>
     </row>
   </sheetData>
@@ -7662,18 +7658,18 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.26953125" customWidth="1"/>
-    <col min="2" max="2" width="105.1796875" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="105.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>151</v>
       </c>
@@ -7681,7 +7677,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -7689,7 +7685,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -7697,7 +7693,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>155</v>
       </c>
@@ -7705,7 +7701,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -7713,7 +7709,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -7721,7 +7717,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -7729,7 +7725,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>161</v>
       </c>
@@ -7737,7 +7733,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>163</v>
       </c>
@@ -7745,7 +7741,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -7753,7 +7749,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -7761,7 +7757,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -7769,7 +7765,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -7777,7 +7773,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -7785,7 +7781,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>170</v>
       </c>
@@ -7793,7 +7789,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -7801,7 +7797,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>174</v>
       </c>
@@ -7809,7 +7805,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>176</v>
       </c>
@@ -8061,6 +8057,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="80b53ead-ac38-442a-b597-5a0e2e0802cd">
@@ -8069,15 +8074,6 @@
     <TaxCatchAll xmlns="5ec1cc48-4270-4222-9ed5-54ce9e59d47b" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8100,6 +8096,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B1B5D08-A2EB-4F47-BA81-DA28AA2A09F4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66AF2240-620B-4312-9739-CAF731E4A98F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8108,12 +8112,4 @@
     <ds:schemaRef ds:uri="5ec1cc48-4270-4222-9ed5-54ce9e59d47b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B1B5D08-A2EB-4F47-BA81-DA28AA2A09F4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>